<commit_message>
.gitignore para airflow/dags/lib/__pycache__/* y mail de destino del resultado del DAG
</commit_message>
<xml_diff>
--- a/airflow/reports/reporte.xlsx
+++ b/airflow/reports/reporte.xlsx
@@ -547,12 +547,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>100GE2/0/0</t>
+          <t>100GE2/1/4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/0</t>
+          <t>IC1.HOR1100GE2/1/4</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/0)</t>
+          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/0)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -600,12 +600,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>100GE2/0/1</t>
+          <t>100GE9/0/0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/1</t>
+          <t>IC1.HOR1100GE9/0/0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -625,10 +625,14 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/1)</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/2) (32WPU01 2/15/C2) Linea:15008585</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Linea:15008585</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>ok</t>
@@ -653,12 +657,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>100GE2/0/2</t>
+          <t>100GE9/0/1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/2</t>
+          <t>IC1.HOR1100GE9/0/1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -678,10 +682,14 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/2)</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/3) (32WPU01 2/15/C1) Linea:15008555</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Linea:15008555</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>ok</t>
@@ -706,12 +714,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>100GE2/0/3</t>
+          <t>100GE9/0/2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/3</t>
+          <t>IC1.HOR1100GE9/0/2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -731,10 +739,14 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/3)</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/4) (32WPU01 1/14/C1) Linea:15008586</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Linea:15008586</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>ok</t>
@@ -759,12 +771,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>100GE2/0/4</t>
+          <t>100GE9/0/3</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/4</t>
+          <t>IC1.HOR1100GE9/0/3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -784,10 +796,14 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/4)</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/5) (32WPU01 1/16/C1) Linea:15008587</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Linea:15008587</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>ok</t>
@@ -812,12 +828,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>100GE2/0/5</t>
+          <t>100GE9/0/4</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/5</t>
+          <t>IC1.HOR1100GE9/0/4</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -837,10 +853,14 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/5)</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/9/0/6)  (32WPU01 1/16/C2) Linea:15008383</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Linea:15008383</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>ok</t>
@@ -865,12 +885,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>100GE2/0/6</t>
+          <t>100GE9/0/5</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/6</t>
+          <t>IC1.HOR1100GE9/0/5</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -890,7 +910,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/6)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/1) (S004_1 98HOR02 5/1)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -918,12 +938,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>100GE2/0/10</t>
+          <t>100GE9/0/6</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/10</t>
+          <t>IC1.HOR1100GE9/0/6</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -943,7 +963,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/0)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/2) (S004_2 98HOR02 5/2)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -971,12 +991,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>100GE2/0/11</t>
+          <t>100GE9/0/7</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/11</t>
+          <t>IC1.HOR1100GE9/0/7</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -996,7 +1016,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/1)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/0) (S004_3 98HOR02 6/1)</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -1024,12 +1044,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>100GE2/0/12</t>
+          <t>100GE9/0/8</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/12</t>
+          <t>IC1.HOR1100GE9/0/8</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1049,7 +1069,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/2)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/1) (S004_4 98HOR02 6/2)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
@@ -1077,12 +1097,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>100GE2/0/13</t>
+          <t>100GE9/0/9</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/13</t>
+          <t>IC1.HOR1100GE9/0/9</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1102,7 +1122,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/3)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/2) (S004_5 98HOR02 7/1)</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -1130,12 +1150,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>100GE2/0/14</t>
+          <t>100GE9/0/10</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/14</t>
+          <t>IC1.HOR1100GE9/0/10</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1155,7 +1175,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/0)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/2) (S004_6 98HOR02 7/2)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -1183,12 +1203,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>100GE2/0/15</t>
+          <t>100GE9/0/11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/15</t>
+          <t>IC1.HOR1100GE9/0/11</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1208,7 +1228,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/1)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/3) (S004_7 98HOR02 8/1)</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -1236,12 +1256,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>100GE2/0/16</t>
+          <t>100GE9/0/12</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/16</t>
+          <t>IC1.HOR1100GE9/0/12</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1261,7 +1281,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/2)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/4) (WDM3.HOR1 2/3/C1)</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
@@ -1289,12 +1309,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>100GE2/0/17</t>
+          <t>100GE9/0/13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/17</t>
+          <t>IC1.HOR1100GE9/0/13</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1314,7 +1334,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/3)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/5) (WDM3.HOR1 4/9/C1)</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -1342,12 +1362,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>100GE2/0/18</t>
+          <t>100GE9/0/14</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/18</t>
+          <t>IC1.HOR1100GE9/0/14</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1367,7 +1387,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/3/0/3)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/6) (WDM3.HOR1 4/11/C1)</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
@@ -1395,12 +1415,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>100GE2/0/19</t>
+          <t>100GE9/0/15</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/19</t>
+          <t>IC1.HOR1100GE9/0/15</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1420,7 +1440,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/0)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/3) (WDM3.HOR1 4/1/C1)</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -1448,12 +1468,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>100GE2/1/0</t>
+          <t>100GE9/0/16</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/0</t>
+          <t>IC1.HOR1100GE9/0/16</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1473,7 +1493,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/4) (WDM3.HOR1 4/3/C1)</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -1501,12 +1521,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>100GE2/1/1</t>
+          <t>100GE9/0/17</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/1</t>
+          <t>IC1.HOR1100GE9/0/17</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1526,7 +1546,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/2)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/5) (WDM3.HOR1 4/4/C1)</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -1554,12 +1574,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>100GE2/1/2</t>
+          <t>100GE9/0/18</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/2</t>
+          <t>IC1.HOR1100GE9/0/18</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1579,7 +1599,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/3)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/8/0/3) (WDM3.HOR1 4/6/C1)</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
@@ -1607,12 +1627,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>100GE2/1/3</t>
+          <t>100GE9/0/19</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/3</t>
+          <t>IC1.HOR1100GE9/0/19</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1632,7 +1652,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/0/0/1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/0/0/11) (WDM3.HOR1 6/8/C2)</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -1660,12 +1680,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>100GE2/1/4</t>
+          <t>100GE9/1/0</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/4</t>
+          <t>IC1.HOR1100GE9/1/0</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1685,7 +1705,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/0)</t>
+          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/0) (S006_1 98HOR01 1C/6/1)</t>
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
@@ -1713,12 +1733,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>100GE2/1/5</t>
+          <t>100GE9/1/1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/5</t>
+          <t>IC1.HOR1100GE9/1/1</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1738,7 +1758,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/1)</t>
+          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/1) (S006_2 98HOR01 1C/6/2)</t>
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
@@ -1766,12 +1786,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>100GE8/0/0</t>
+          <t>100GE9/1/2</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/0</t>
+          <t>IC1.HOR1100GE9/1/2</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1791,7 +1811,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/0) (S3-005 88HOR02 0/3/1) Linea:11004841</t>
+          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/1/0) (S006_3 98HOR01 1C/7/1)</t>
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
@@ -1819,12 +1839,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>100GE8/0/1</t>
+          <t>100GE9/1/3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/1</t>
+          <t>IC1.HOR1100GE9/1/3</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1844,10 +1864,14 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/1) (S3-004 88HOR01 0/3/1) Linea:11004840</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr"/>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/0) (S004_8 98HOR02 8/2) Linea:15009213</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Linea:15009213</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr">
         <is>
           <t>ok</t>
@@ -1872,12 +1896,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>100GE8/0/2</t>
+          <t>100GE9/1/4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/2</t>
+          <t>IC1.HOR1100GE9/1/4</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1897,10 +1921,14 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/2) (S3-002 88HOR01 0/12/1) Linea:15003692</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr"/>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/1) (S004_9 98HOR02 14/1) Linea:15009214</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Linea:15009214</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
           <t>ok</t>
@@ -1925,12 +1953,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>100GE8/0/3</t>
+          <t>100GE9/1/5</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/3</t>
+          <t>IC1.HOR1100GE9/1/5</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1950,10 +1978,14 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/5/0/0) (S3-001 88HOR02 0/16/1) Linea:15003451</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr"/>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/2) (S004_10 98HOR02 14/2) Linea:15009215</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Linea:15009215</t>
+        </is>
+      </c>
       <c r="K28" t="inlineStr">
         <is>
           <t>ok</t>
@@ -1978,12 +2010,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>100GE9/0/0</t>
+          <t>100GE9/1/6</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/0</t>
+          <t>IC1.HOR1100GE9/1/6</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2003,12 +2035,12 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/2) (32WPU01 2/15/C2) Linea:15008585</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/2) (98HOR01 3/1) Linea: 15009094</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Linea:15008585</t>
+          <t>Linea: 15009094</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2035,12 +2067,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>100GE9/0/1</t>
+          <t>100GE9/1/7</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/1</t>
+          <t>IC1.HOR1100GE9/1/7</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2060,12 +2092,12 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/3) (32WPU01 2/15/C1) Linea:15008555</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/3) (98HOR01 3/2) Linea: 15009095</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Linea:15008555</t>
+          <t>Linea: 15009095</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2092,12 +2124,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>100GE9/0/2</t>
+          <t>100GE9/1/8</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/2</t>
+          <t>IC1.HOR1100GE9/1/8</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2117,12 +2149,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/4) (32WPU01 1/14/C1) Linea:15008586</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/4) (98HOR01 5/1) Linea: 15009096</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Linea:15008586</t>
+          <t>Linea: 15009096 - BEL1NA</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2149,12 +2181,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>100GE9/0/3</t>
+          <t>100GE9/1/9</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/3</t>
+          <t>IC1.HOR1100GE9/1/9</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2174,12 +2206,12 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/5) (32WPU01 1/16/C1) Linea:15008587</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/5) (98HOR01 5/2) Linea: 15009097</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Linea:15008587</t>
+          <t>Linea: 15009097 - BEL1NA</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2206,12 +2238,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>100GE9/0/4</t>
+          <t>100GE9/1/10</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/4</t>
+          <t>IC1.HOR1100GE9/1/10</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2231,12 +2263,12 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/9/0/6)  (32WPU01 1/16/C2) Linea:15008383</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/6) (98HOR01 4/1) Linea: 15009098</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Linea:15008383</t>
+          <t>Linea: 15009098</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2263,12 +2295,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>100GE9/0/5</t>
+          <t>100GE2/0/0</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/5</t>
+          <t>IC1.HOR1100GE2/0/0</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2288,7 +2320,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/1) (S004_1 98HOR02 5/1)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/0)</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
@@ -2316,12 +2348,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>100GE9/0/6</t>
+          <t>100GE2/0/1</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/6</t>
+          <t>IC1.HOR1100GE2/0/1</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2341,7 +2373,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/2) (S004_2 98HOR02 5/2)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/1)</t>
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
@@ -2369,12 +2401,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>100GE9/0/7</t>
+          <t>100GE2/0/2</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/7</t>
+          <t>IC1.HOR1100GE2/0/2</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2394,7 +2426,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/0) (S004_3 98HOR02 6/1)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/2)</t>
         </is>
       </c>
       <c r="J36" t="inlineStr"/>
@@ -2422,12 +2454,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>100GE9/0/8</t>
+          <t>100GE2/0/3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/8</t>
+          <t>IC1.HOR1100GE2/0/3</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2447,7 +2479,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/1) (S004_4 98HOR02 6/2)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/3)</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
@@ -2475,12 +2507,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>100GE9/0/9</t>
+          <t>100GE2/0/4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/9</t>
+          <t>IC1.HOR1100GE2/0/4</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2500,7 +2532,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/2) (S004_5 98HOR02 7/1)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/4)</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
@@ -2528,12 +2560,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>100GE9/0/10</t>
+          <t>100GE2/0/5</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/10</t>
+          <t>IC1.HOR1100GE2/0/5</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2553,7 +2585,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/2) (S004_6 98HOR02 7/2)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/5)</t>
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
@@ -2581,12 +2613,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>100GE9/0/11</t>
+          <t>100GE2/0/6</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/11</t>
+          <t>IC1.HOR1100GE2/0/6</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2606,7 +2638,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/3) (S004_7 98HOR02 8/1)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/6)</t>
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
@@ -2634,12 +2666,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>100GE9/0/12</t>
+          <t>100GE2/0/10</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/12</t>
+          <t>IC1.HOR1100GE2/0/10</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2659,7 +2691,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/4) (WDM3.HOR1 2/3/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/0)</t>
         </is>
       </c>
       <c r="J41" t="inlineStr"/>
@@ -2687,12 +2719,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>100GE9/0/13</t>
+          <t>100GE2/0/11</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/13</t>
+          <t>IC1.HOR1100GE2/0/11</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2712,7 +2744,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/5) (WDM3.HOR1 4/9/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/1)</t>
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
@@ -2740,12 +2772,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>100GE9/0/14</t>
+          <t>100GE2/0/12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/14</t>
+          <t>IC1.HOR1100GE2/0/12</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2765,7 +2797,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/6) (WDM3.HOR1 4/11/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/2)</t>
         </is>
       </c>
       <c r="J43" t="inlineStr"/>
@@ -2793,12 +2825,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>100GE9/0/15</t>
+          <t>100GE2/0/13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/15</t>
+          <t>IC1.HOR1100GE2/0/13</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2818,7 +2850,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/3) (WDM3.HOR1 4/1/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/3)</t>
         </is>
       </c>
       <c r="J44" t="inlineStr"/>
@@ -2846,12 +2878,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>100GE9/0/16</t>
+          <t>100GE2/0/14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/16</t>
+          <t>IC1.HOR1100GE2/0/14</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2871,7 +2903,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/4) (WDM3.HOR1 4/3/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/0)</t>
         </is>
       </c>
       <c r="J45" t="inlineStr"/>
@@ -2899,12 +2931,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>100GE9/0/17</t>
+          <t>100GE2/0/15</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/17</t>
+          <t>IC1.HOR1100GE2/0/15</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2924,7 +2956,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/5) (WDM3.HOR1 4/4/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/1)</t>
         </is>
       </c>
       <c r="J46" t="inlineStr"/>
@@ -2952,12 +2984,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>100GE9/0/18</t>
+          <t>100GE2/0/16</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/18</t>
+          <t>IC1.HOR1100GE2/0/16</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2977,7 +3009,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/8/0/3) (WDM3.HOR1 4/6/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/2)</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -3005,12 +3037,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>100GE9/0/19</t>
+          <t>100GE2/0/17</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/19</t>
+          <t>IC1.HOR1100GE2/0/17</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3030,7 +3062,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/0/0/11) (WDM3.HOR1 6/8/C2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/3)</t>
         </is>
       </c>
       <c r="J48" t="inlineStr"/>
@@ -3058,12 +3090,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>100GE9/1/0</t>
+          <t>100GE2/0/18</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/0</t>
+          <t>IC1.HOR1100GE2/0/18</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -3083,7 +3115,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/0) (S006_1 98HOR01 1C/6/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/3/0/3)</t>
         </is>
       </c>
       <c r="J49" t="inlineStr"/>
@@ -3111,12 +3143,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>100GE9/1/1</t>
+          <t>100GE2/0/19</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/1</t>
+          <t>IC1.HOR1100GE2/0/19</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3136,7 +3168,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/1) (S006_2 98HOR01 1C/6/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/0)</t>
         </is>
       </c>
       <c r="J50" t="inlineStr"/>
@@ -3164,12 +3196,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>100GE9/1/2</t>
+          <t>100GE2/1/0</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/2</t>
+          <t>IC1.HOR1100GE2/1/0</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -3189,7 +3221,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/1/0) (S006_3 98HOR01 1C/7/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/1)</t>
         </is>
       </c>
       <c r="J51" t="inlineStr"/>
@@ -3217,12 +3249,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>100GE9/1/3</t>
+          <t>100GE2/1/1</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/3</t>
+          <t>IC1.HOR1100GE2/1/1</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -3242,14 +3274,10 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/0) (S004_8 98HOR02 8/2) Linea:15009213</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Linea:15009213</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/2)</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3274,12 +3302,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>100GE9/1/4</t>
+          <t>100GE2/1/2</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/4</t>
+          <t>IC1.HOR1100GE2/1/2</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -3299,14 +3327,10 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/1) (S004_9 98HOR02 14/1) Linea:15009214</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>Linea:15009214</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/3)</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3331,12 +3355,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>100GE9/1/5</t>
+          <t>100GE2/1/3</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/5</t>
+          <t>IC1.HOR1100GE2/1/3</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -3356,14 +3380,10 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/2) (S004_10 98HOR02 14/2) Linea:15009215</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>Linea:15009215</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/0/0/1)</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3388,12 +3408,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>100GE9/1/6</t>
+          <t>100GE2/1/5</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/6</t>
+          <t>IC1.HOR1100GE2/1/5</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -3413,14 +3433,10 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/2) (98HOR01 3/1) Linea: 15009094</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Linea: 15009094</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/1)</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3445,12 +3461,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>100GE9/1/7</t>
+          <t>100GE8/0/0</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/7</t>
+          <t>IC1.HOR1100GE8/0/0</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -3470,14 +3486,10 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/3) (98HOR01 3/2) Linea: 15009095</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>Linea: 15009095</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/0) (S3-005 88HOR02 0/3/1) Linea:11004841</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3502,12 +3514,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>100GE9/1/8</t>
+          <t>100GE8/0/1</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/8</t>
+          <t>IC1.HOR1100GE8/0/1</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -3527,14 +3539,10 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/4) (98HOR01 5/1) Linea: 15009096</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>Linea: 15009096 - BEL1NA</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/1) (S3-004 88HOR01 0/3/1) Linea:11004840</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3559,12 +3567,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>100GE9/1/9</t>
+          <t>100GE8/0/2</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/9</t>
+          <t>IC1.HOR1100GE8/0/2</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -3584,14 +3592,10 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/5) (98HOR01 5/2) Linea: 15009097</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Linea: 15009097 - BEL1NA</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/2) (S3-002 88HOR01 0/12/1) Linea:15003692</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3616,12 +3620,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>100GE9/1/10</t>
+          <t>100GE8/0/3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/10</t>
+          <t>IC1.HOR1100GE8/0/3</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -3641,14 +3645,10 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/6) (98HOR01 4/1) Linea: 15009098</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>Linea: 15009098</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:IRD1NA (Hu0/5/0/0) (S3-001 88HOR02 0/16/1) Linea:15003451</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3673,12 +3673,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>100GE2/0/8</t>
+          <t>100GE8/1/7</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/8</t>
+          <t>IC1.HOR1100GE8/1/7</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -3722,12 +3722,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>100GE2/0/9</t>
+          <t>100GE8/1/8</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/9</t>
+          <t>IC1.HOR1100GE8/1/8</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -3771,12 +3771,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>100GE2/1/6</t>
+          <t>100GE8/1/9</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/6</t>
+          <t>IC1.HOR1100GE8/1/9</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -3820,12 +3820,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>100GE2/1/14</t>
+          <t>100GE8/1/10</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/14</t>
+          <t>IC1.HOR1100GE8/1/10</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3869,12 +3869,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>100GE2/1/15</t>
+          <t>100GE8/1/11</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/15</t>
+          <t>IC1.HOR1100GE8/1/11</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3918,12 +3918,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>100GE2/1/16</t>
+          <t>100GE8/1/12</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/16</t>
+          <t>IC1.HOR1100GE8/1/12</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3967,12 +3967,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>100GE2/1/17</t>
+          <t>100GE8/1/13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/17</t>
+          <t>IC1.HOR1100GE8/1/13</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -4016,12 +4016,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>100GE2/1/18</t>
+          <t>100GE8/1/14</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/18</t>
+          <t>IC1.HOR1100GE8/1/14</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -4065,12 +4065,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>100GE2/1/19</t>
+          <t>100GE8/1/15</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/19</t>
+          <t>IC1.HOR1100GE8/1/15</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -4114,12 +4114,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>100GE3/0/7</t>
+          <t>100GE8/1/16</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/7</t>
+          <t>IC1.HOR1100GE8/1/16</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -4163,12 +4163,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>100GE3/0/8</t>
+          <t>100GE8/1/17</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/8</t>
+          <t>IC1.HOR1100GE8/1/17</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -4212,12 +4212,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>100GE3/0/9</t>
+          <t>100GE8/1/18</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/9</t>
+          <t>IC1.HOR1100GE8/1/18</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -4261,12 +4261,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>100GE3/0/10</t>
+          <t>100GE8/1/19</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/10</t>
+          <t>IC1.HOR1100GE8/1/19</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -4310,12 +4310,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>100GE3/0/11</t>
+          <t>100GE9/1/11</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/11</t>
+          <t>IC1.HOR1100GE9/1/11</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -4359,12 +4359,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>100GE3/0/12</t>
+          <t>100GE9/1/12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/12</t>
+          <t>IC1.HOR1100GE9/1/12</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -4408,12 +4408,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>100GE3/0/13</t>
+          <t>100GE9/1/13</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/13</t>
+          <t>IC1.HOR1100GE9/1/13</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -4457,12 +4457,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>100GE3/0/14</t>
+          <t>100GE9/1/14</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/14</t>
+          <t>IC1.HOR1100GE9/1/14</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -4506,12 +4506,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>100GE3/0/15</t>
+          <t>100GE9/1/15</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/15</t>
+          <t>IC1.HOR1100GE9/1/15</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -4555,12 +4555,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>100GE3/0/16</t>
+          <t>100GE9/1/16</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/16</t>
+          <t>IC1.HOR1100GE9/1/16</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -4604,12 +4604,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>100GE3/0/17</t>
+          <t>100GE9/1/17</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/17</t>
+          <t>IC1.HOR1100GE9/1/17</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -4653,12 +4653,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>100GE3/0/18</t>
+          <t>100GE9/1/18</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/18</t>
+          <t>IC1.HOR1100GE9/1/18</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -4702,12 +4702,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>100GE3/0/19</t>
+          <t>100GE9/1/19</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/19</t>
+          <t>IC1.HOR1100GE9/1/19</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -4751,12 +4751,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>100GE3/1/0</t>
+          <t>100GE2/0/8</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/0</t>
+          <t>IC1.HOR1100GE2/0/8</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -4800,12 +4800,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>100GE3/1/1</t>
+          <t>100GE2/0/9</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/1</t>
+          <t>IC1.HOR1100GE2/0/9</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -4849,17 +4849,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>100GE3/1/2</t>
+          <t>GE10/0/26(100M)</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/2</t>
+          <t>IC1.HOR1GE10/0/26(100M)</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>100GE</t>
+          <t>GE</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -4898,12 +4898,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>100GE3/1/3</t>
+          <t>100GE2/1/6</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/3</t>
+          <t>IC1.HOR1100GE2/1/6</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -4947,12 +4947,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>100GE3/1/4</t>
+          <t>100GE2/1/14</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/4</t>
+          <t>IC1.HOR1100GE2/1/14</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -4996,12 +4996,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>100GE3/1/5</t>
+          <t>100GE2/1/15</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/5</t>
+          <t>IC1.HOR1100GE2/1/15</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -5045,12 +5045,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>100GE3/1/6</t>
+          <t>100GE2/1/16</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/6</t>
+          <t>IC1.HOR1100GE2/1/16</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -5094,12 +5094,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>100GE3/1/7</t>
+          <t>100GE2/1/17</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/7</t>
+          <t>IC1.HOR1100GE2/1/17</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -5143,12 +5143,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>100GE3/1/8</t>
+          <t>100GE2/1/18</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/8</t>
+          <t>IC1.HOR1100GE2/1/18</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -5192,12 +5192,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>100GE3/1/9</t>
+          <t>100GE2/1/19</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/9</t>
+          <t>IC1.HOR1100GE2/1/19</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -5241,12 +5241,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>100GE3/1/10</t>
+          <t>100GE3/0/7</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/10</t>
+          <t>IC1.HOR1100GE3/0/7</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -5290,12 +5290,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>100GE3/1/11</t>
+          <t>100GE3/0/8</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/11</t>
+          <t>IC1.HOR1100GE3/0/8</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -5339,12 +5339,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>100GE3/1/12</t>
+          <t>100GE3/0/9</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/12</t>
+          <t>IC1.HOR1100GE3/0/9</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -5388,12 +5388,12 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>100GE3/1/13</t>
+          <t>100GE3/0/10</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/13</t>
+          <t>IC1.HOR1100GE3/0/10</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -5437,12 +5437,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>100GE3/1/14</t>
+          <t>100GE3/0/11</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/14</t>
+          <t>IC1.HOR1100GE3/0/11</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -5486,12 +5486,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>100GE3/1/15</t>
+          <t>100GE3/0/12</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/15</t>
+          <t>IC1.HOR1100GE3/0/12</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -5535,12 +5535,12 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>100GE3/1/16</t>
+          <t>100GE3/0/13</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/16</t>
+          <t>IC1.HOR1100GE3/0/13</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -5584,12 +5584,12 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>100GE3/1/17</t>
+          <t>100GE3/0/14</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/17</t>
+          <t>IC1.HOR1100GE3/0/14</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -5633,12 +5633,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>100GE3/1/18</t>
+          <t>100GE3/0/15</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/18</t>
+          <t>IC1.HOR1100GE3/0/15</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -5682,12 +5682,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>100GE3/1/19</t>
+          <t>100GE3/0/16</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/19</t>
+          <t>IC1.HOR1100GE3/0/16</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -5731,12 +5731,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>100GE8/0/9</t>
+          <t>100GE3/0/17</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/9</t>
+          <t>IC1.HOR1100GE3/0/17</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -5780,12 +5780,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>100GE8/0/10</t>
+          <t>100GE3/0/18</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/10</t>
+          <t>IC1.HOR1100GE3/0/18</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -5829,12 +5829,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>100GE8/0/11</t>
+          <t>100GE3/0/19</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/11</t>
+          <t>IC1.HOR1100GE3/0/19</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -5878,12 +5878,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>100GE8/0/12</t>
+          <t>100GE3/1/0</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/12</t>
+          <t>IC1.HOR1100GE3/1/0</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -5927,12 +5927,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>100GE8/0/13</t>
+          <t>100GE3/1/1</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/13</t>
+          <t>IC1.HOR1100GE3/1/1</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -5976,12 +5976,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>100GE8/0/14</t>
+          <t>100GE3/1/2</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/14</t>
+          <t>IC1.HOR1100GE3/1/2</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -6025,12 +6025,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>100GE8/0/15</t>
+          <t>100GE3/1/3</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/15</t>
+          <t>IC1.HOR1100GE3/1/3</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -6074,12 +6074,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>100GE8/0/16</t>
+          <t>100GE3/1/4</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/16</t>
+          <t>IC1.HOR1100GE3/1/4</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -6123,12 +6123,12 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>100GE8/0/17</t>
+          <t>100GE3/1/5</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/17</t>
+          <t>IC1.HOR1100GE3/1/5</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -6172,12 +6172,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>100GE8/0/18</t>
+          <t>100GE3/1/6</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/18</t>
+          <t>IC1.HOR1100GE3/1/6</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -6221,12 +6221,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>100GE8/0/19</t>
+          <t>100GE3/1/7</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/19</t>
+          <t>IC1.HOR1100GE3/1/7</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -6270,12 +6270,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>100GE8/1/0</t>
+          <t>100GE3/1/8</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/0</t>
+          <t>IC1.HOR1100GE3/1/8</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -6319,12 +6319,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>100GE8/1/1</t>
+          <t>100GE3/1/9</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/1</t>
+          <t>IC1.HOR1100GE3/1/9</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -6368,12 +6368,12 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>100GE8/1/2</t>
+          <t>100GE3/1/10</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/2</t>
+          <t>IC1.HOR1100GE3/1/10</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -6417,12 +6417,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>100GE8/1/3</t>
+          <t>100GE3/1/11</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/3</t>
+          <t>IC1.HOR1100GE3/1/11</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -6466,12 +6466,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>100GE8/1/4</t>
+          <t>100GE3/1/12</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/4</t>
+          <t>IC1.HOR1100GE3/1/12</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -6515,12 +6515,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>100GE8/1/5</t>
+          <t>100GE3/1/13</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/5</t>
+          <t>IC1.HOR1100GE3/1/13</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -6564,12 +6564,12 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>100GE8/1/6</t>
+          <t>100GE3/1/14</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/6</t>
+          <t>IC1.HOR1100GE3/1/14</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -6613,12 +6613,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>100GE8/1/7</t>
+          <t>100GE3/1/15</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/7</t>
+          <t>IC1.HOR1100GE3/1/15</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -6662,12 +6662,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>100GE8/1/8</t>
+          <t>100GE3/1/16</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/8</t>
+          <t>IC1.HOR1100GE3/1/16</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -6711,12 +6711,12 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>100GE8/1/9</t>
+          <t>100GE3/1/17</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/9</t>
+          <t>IC1.HOR1100GE3/1/17</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -6760,12 +6760,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>100GE8/1/10</t>
+          <t>100GE3/1/18</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/10</t>
+          <t>IC1.HOR1100GE3/1/18</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -6809,12 +6809,12 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>100GE8/1/11</t>
+          <t>100GE3/1/19</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/11</t>
+          <t>IC1.HOR1100GE3/1/19</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -6858,12 +6858,12 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>100GE8/1/12</t>
+          <t>100GE8/0/9</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/12</t>
+          <t>IC1.HOR1100GE8/0/9</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -6907,12 +6907,12 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>100GE8/1/13</t>
+          <t>100GE8/0/10</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/13</t>
+          <t>IC1.HOR1100GE8/0/10</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -6956,12 +6956,12 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>100GE8/1/14</t>
+          <t>100GE8/0/11</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/14</t>
+          <t>IC1.HOR1100GE8/0/11</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -7005,12 +7005,12 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>100GE8/1/15</t>
+          <t>100GE8/0/12</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/15</t>
+          <t>IC1.HOR1100GE8/0/12</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -7054,12 +7054,12 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>100GE8/1/16</t>
+          <t>100GE8/0/13</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/16</t>
+          <t>IC1.HOR1100GE8/0/13</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -7103,12 +7103,12 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>100GE8/1/17</t>
+          <t>100GE8/0/14</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/17</t>
+          <t>IC1.HOR1100GE8/0/14</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -7152,12 +7152,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>100GE8/1/18</t>
+          <t>100GE8/0/15</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/18</t>
+          <t>IC1.HOR1100GE8/0/15</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -7201,12 +7201,12 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>100GE8/1/19</t>
+          <t>100GE8/0/16</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/19</t>
+          <t>IC1.HOR1100GE8/0/16</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -7250,12 +7250,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>100GE9/1/11</t>
+          <t>100GE8/0/17</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/11</t>
+          <t>IC1.HOR1100GE8/0/17</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -7299,12 +7299,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>100GE9/1/12</t>
+          <t>100GE8/0/18</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/12</t>
+          <t>IC1.HOR1100GE8/0/18</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -7348,12 +7348,12 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>100GE9/1/13</t>
+          <t>100GE8/0/19</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/13</t>
+          <t>IC1.HOR1100GE8/0/19</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -7397,12 +7397,12 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>100GE9/1/14</t>
+          <t>100GE8/1/0</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/14</t>
+          <t>IC1.HOR1100GE8/1/0</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -7446,12 +7446,12 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>100GE9/1/15</t>
+          <t>100GE8/1/1</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/15</t>
+          <t>IC1.HOR1100GE8/1/1</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -7495,12 +7495,12 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>100GE9/1/16</t>
+          <t>100GE8/1/2</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/16</t>
+          <t>IC1.HOR1100GE8/1/2</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -7544,12 +7544,12 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>100GE9/1/17</t>
+          <t>100GE8/1/3</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/17</t>
+          <t>IC1.HOR1100GE8/1/3</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -7593,12 +7593,12 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>100GE9/1/18</t>
+          <t>100GE8/1/4</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/18</t>
+          <t>IC1.HOR1100GE8/1/4</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -7642,12 +7642,12 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>100GE9/1/19</t>
+          <t>100GE8/1/5</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/19</t>
+          <t>IC1.HOR1100GE8/1/5</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -7691,17 +7691,17 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>GE1/0/0(100M)</t>
+          <t>100GE8/1/6</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/0(100M)</t>
+          <t>IC1.HOR1100GE8/1/6</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>100GE</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
@@ -7740,12 +7740,12 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>GE1/0/1(100M)</t>
+          <t>GE1/0/0(100M)</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/1(100M)</t>
+          <t>IC1.HOR1GE1/0/0(100M)</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -7789,12 +7789,12 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>GE1/0/2(100M)</t>
+          <t>GE1/0/1(100M)</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/2(100M)</t>
+          <t>IC1.HOR1GE1/0/1(100M)</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -7838,12 +7838,12 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>GE1/0/3(100M)</t>
+          <t>GE1/0/2(100M)</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/3(100M)</t>
+          <t>IC1.HOR1GE1/0/2(100M)</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -7887,12 +7887,12 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>GE1/0/4(100M)</t>
+          <t>GE1/0/3(100M)</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/4(100M)</t>
+          <t>IC1.HOR1GE1/0/3(100M)</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -7936,12 +7936,12 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>GE1/0/5(100M)</t>
+          <t>GE1/0/4(100M)</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/5(100M)</t>
+          <t>IC1.HOR1GE1/0/4(100M)</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -7985,12 +7985,12 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>GE1/0/6(100M)</t>
+          <t>GE1/0/5(100M)</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/6(100M)</t>
+          <t>IC1.HOR1GE1/0/5(100M)</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -8034,12 +8034,12 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>GE1/0/7(100M)</t>
+          <t>GE1/0/6(100M)</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/7(100M)</t>
+          <t>IC1.HOR1GE1/0/6(100M)</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -8083,12 +8083,12 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>GE1/0/8(100M)</t>
+          <t>GE1/0/7(100M)</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/8(100M)</t>
+          <t>IC1.HOR1GE1/0/7(100M)</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -8132,12 +8132,12 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>GE1/0/9(100M)</t>
+          <t>GE1/0/8(100M)</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/9(100M)</t>
+          <t>IC1.HOR1GE1/0/8(100M)</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -8181,12 +8181,12 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>GE1/0/10(100M)</t>
+          <t>GE1/0/9(100M)</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/10(100M)</t>
+          <t>IC1.HOR1GE1/0/9(100M)</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -8230,12 +8230,12 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>GE1/0/11(100M)</t>
+          <t>GE1/0/10(100M)</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/11(100M)</t>
+          <t>IC1.HOR1GE1/0/10(100M)</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -8279,12 +8279,12 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>GE1/0/12(100M)</t>
+          <t>GE1/0/11(100M)</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/12(100M)</t>
+          <t>IC1.HOR1GE1/0/11(100M)</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -8328,12 +8328,12 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>GE1/0/13(100M)</t>
+          <t>GE1/0/12(100M)</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/13(100M)</t>
+          <t>IC1.HOR1GE1/0/12(100M)</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -8377,12 +8377,12 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>GE1/0/14(100M)</t>
+          <t>GE1/0/13(100M)</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/14(100M)</t>
+          <t>IC1.HOR1GE1/0/13(100M)</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -8426,12 +8426,12 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>GE1/0/15(100M)</t>
+          <t>GE1/0/14(100M)</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/15(100M)</t>
+          <t>IC1.HOR1GE1/0/14(100M)</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -8475,12 +8475,12 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>GE1/0/16(100M)</t>
+          <t>GE1/0/15(100M)</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/16(100M)</t>
+          <t>IC1.HOR1GE1/0/15(100M)</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -8524,12 +8524,12 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>GE1/0/17(100M)</t>
+          <t>GE1/0/16(100M)</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/17(100M)</t>
+          <t>IC1.HOR1GE1/0/16(100M)</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -8573,12 +8573,12 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>GE1/0/18(100M)</t>
+          <t>GE1/0/17(100M)</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/18(100M)</t>
+          <t>IC1.HOR1GE1/0/17(100M)</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -8622,12 +8622,12 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>GE1/0/19(100M)</t>
+          <t>GE1/0/18(100M)</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/19(100M)</t>
+          <t>IC1.HOR1GE1/0/18(100M)</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -8671,12 +8671,12 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>GE1/0/20(100M)</t>
+          <t>GE1/0/19(100M)</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/20(100M)</t>
+          <t>IC1.HOR1GE1/0/19(100M)</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -8720,12 +8720,12 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>GE1/0/21(100M)</t>
+          <t>GE1/0/20(100M)</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/21(100M)</t>
+          <t>IC1.HOR1GE1/0/20(100M)</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -8769,12 +8769,12 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>GE1/0/22(100M)</t>
+          <t>GE1/0/21(100M)</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/22(100M)</t>
+          <t>IC1.HOR1GE1/0/21(100M)</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -8818,12 +8818,12 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>GE1/0/23(100M)</t>
+          <t>GE1/0/22(100M)</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/23(100M)</t>
+          <t>IC1.HOR1GE1/0/22(100M)</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -8867,12 +8867,12 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>GE1/0/24(100M)</t>
+          <t>GE1/0/23(100M)</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/24(100M)</t>
+          <t>IC1.HOR1GE1/0/23(100M)</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -8916,12 +8916,12 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>GE1/0/25(100M)</t>
+          <t>GE1/0/24(100M)</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/25(100M)</t>
+          <t>IC1.HOR1GE1/0/24(100M)</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -8965,12 +8965,12 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>GE1/0/26(100M)</t>
+          <t>GE1/0/25(100M)</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/26(100M)</t>
+          <t>IC1.HOR1GE1/0/25(100M)</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -9014,12 +9014,12 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>GE1/0/27(100M)</t>
+          <t>GE1/0/26(100M)</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/27(100M)</t>
+          <t>IC1.HOR1GE1/0/26(100M)</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -9063,12 +9063,12 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>GE1/0/28(100M)</t>
+          <t>GE1/0/27(100M)</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/28(100M)</t>
+          <t>IC1.HOR1GE1/0/27(100M)</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -9112,12 +9112,12 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>GE1/0/29(100M)</t>
+          <t>GE1/0/28(100M)</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/29(100M)</t>
+          <t>IC1.HOR1GE1/0/28(100M)</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -9161,12 +9161,12 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>GE1/0/30(100M)</t>
+          <t>GE1/0/29(100M)</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/30(100M)</t>
+          <t>IC1.HOR1GE1/0/29(100M)</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -9210,12 +9210,12 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>GE1/0/31(100M)</t>
+          <t>GE1/0/30(100M)</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/31(100M)</t>
+          <t>IC1.HOR1GE1/0/30(100M)</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -9259,12 +9259,12 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>GE1/0/32(100M)</t>
+          <t>GE1/0/31(100M)</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/32(100M)</t>
+          <t>IC1.HOR1GE1/0/31(100M)</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -9308,12 +9308,12 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>GE1/0/33(100M)</t>
+          <t>GE1/0/32(100M)</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/33(100M)</t>
+          <t>IC1.HOR1GE1/0/32(100M)</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -9357,12 +9357,12 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>GE1/0/34(100M)</t>
+          <t>GE1/0/33(100M)</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/34(100M)</t>
+          <t>IC1.HOR1GE1/0/33(100M)</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -9406,12 +9406,12 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>GE1/0/35(100M)</t>
+          <t>GE1/0/34(100M)</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/35(100M)</t>
+          <t>IC1.HOR1GE1/0/34(100M)</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -9455,12 +9455,12 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>GE1/0/36(100M)</t>
+          <t>GE1/0/35(100M)</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/36(100M)</t>
+          <t>IC1.HOR1GE1/0/35(100M)</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -9504,12 +9504,12 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>GE1/0/37(100M)</t>
+          <t>GE1/0/36(100M)</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/37(100M)</t>
+          <t>IC1.HOR1GE1/0/36(100M)</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -9553,12 +9553,12 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>GE1/0/38(100M)</t>
+          <t>GE1/0/37(100M)</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/38(100M)</t>
+          <t>IC1.HOR1GE1/0/37(100M)</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -9602,12 +9602,12 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>GE1/0/39(100M)</t>
+          <t>GE1/0/38(100M)</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/39(100M)</t>
+          <t>IC1.HOR1GE1/0/38(100M)</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -9651,12 +9651,12 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>GE1/0/40(100M)</t>
+          <t>GE1/0/39(100M)</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/40(100M)</t>
+          <t>IC1.HOR1GE1/0/39(100M)</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -9700,12 +9700,12 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>GE1/0/41(100M)</t>
+          <t>GE1/0/40(100M)</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/41(100M)</t>
+          <t>IC1.HOR1GE1/0/40(100M)</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -9749,12 +9749,12 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>GE1/0/42(100M)</t>
+          <t>GE1/0/41(100M)</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/42(100M)</t>
+          <t>IC1.HOR1GE1/0/41(100M)</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -9798,12 +9798,12 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>GE1/0/43(100M)</t>
+          <t>GE1/0/42(100M)</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/43(100M)</t>
+          <t>IC1.HOR1GE1/0/42(100M)</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -9847,12 +9847,12 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>GE1/0/44(100M)</t>
+          <t>GE1/0/43(100M)</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/44(100M)</t>
+          <t>IC1.HOR1GE1/0/43(100M)</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -9896,12 +9896,12 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>GE1/0/45(100M)</t>
+          <t>GE1/0/44(100M)</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/45(100M)</t>
+          <t>IC1.HOR1GE1/0/44(100M)</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -9945,12 +9945,12 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>GE1/0/46(100M)</t>
+          <t>GE1/0/45(100M)</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/46(100M)</t>
+          <t>IC1.HOR1GE1/0/45(100M)</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -9994,12 +9994,12 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>GE1/0/47(100M)</t>
+          <t>GE1/0/46(100M)</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/47(100M)</t>
+          <t>IC1.HOR1GE1/0/46(100M)</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -10043,12 +10043,12 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>GE1/0/48(100M)</t>
+          <t>GE1/0/47(100M)</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/48(100M)</t>
+          <t>IC1.HOR1GE1/0/47(100M)</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -10092,12 +10092,12 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>GE1/0/49(100M)</t>
+          <t>GE1/0/48(100M)</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/49(100M)</t>
+          <t>IC1.HOR1GE1/0/48(100M)</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -10141,12 +10141,12 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>GE1/0/50(100M)</t>
+          <t>GE1/0/49(100M)</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/50(100M)</t>
+          <t>IC1.HOR1GE1/0/49(100M)</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -10190,12 +10190,12 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>GE1/0/51(100M)</t>
+          <t>GE1/0/50(100M)</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/51(100M)</t>
+          <t>IC1.HOR1GE1/0/50(100M)</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -10239,12 +10239,12 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>GE1/0/52(100M)</t>
+          <t>GE1/0/51(100M)</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/52(100M)</t>
+          <t>IC1.HOR1GE1/0/51(100M)</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -10288,12 +10288,12 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>GE1/0/53(100M)</t>
+          <t>GE1/0/52(100M)</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/53(100M)</t>
+          <t>IC1.HOR1GE1/0/52(100M)</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -10337,12 +10337,12 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>GE1/0/54(100M)</t>
+          <t>GE1/0/53(100M)</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/54(100M)</t>
+          <t>IC1.HOR1GE1/0/53(100M)</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -10386,12 +10386,12 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>GE1/0/55(100M)</t>
+          <t>GE1/0/54(100M)</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/55(100M)</t>
+          <t>IC1.HOR1GE1/0/54(100M)</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -10435,12 +10435,12 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>GE1/0/56(100M)</t>
+          <t>GE1/0/55(100M)</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/56(100M)</t>
+          <t>IC1.HOR1GE1/0/55(100M)</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -10484,12 +10484,12 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>GE1/0/57(100M)</t>
+          <t>GE1/0/56(100M)</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/57(100M)</t>
+          <t>IC1.HOR1GE1/0/56(100M)</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -10533,12 +10533,12 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>GE1/0/58(100M)</t>
+          <t>GE1/0/57(100M)</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/58(100M)</t>
+          <t>IC1.HOR1GE1/0/57(100M)</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -10582,12 +10582,12 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>GE1/0/59(100M)</t>
+          <t>GE1/0/58(100M)</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/59(100M)</t>
+          <t>IC1.HOR1GE1/0/58(100M)</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -10631,12 +10631,12 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>GE10/0/0(100M)</t>
+          <t>GE1/0/59(100M)</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/0(100M)</t>
+          <t>IC1.HOR1GE1/0/59(100M)</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -10680,12 +10680,12 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>GE10/0/1(100M)</t>
+          <t>GE10/0/0(100M)</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/1(100M)</t>
+          <t>IC1.HOR1GE10/0/0(100M)</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -10729,12 +10729,12 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>GE10/0/2(100M)</t>
+          <t>GE10/0/1(100M)</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/2(100M)</t>
+          <t>IC1.HOR1GE10/0/1(100M)</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -10778,12 +10778,12 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>GE10/0/3(100M)</t>
+          <t>GE10/0/2(100M)</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/3(100M)</t>
+          <t>IC1.HOR1GE10/0/2(100M)</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -10827,12 +10827,12 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>GE10/0/4(100M)</t>
+          <t>GE10/0/3(100M)</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/4(100M)</t>
+          <t>IC1.HOR1GE10/0/3(100M)</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -10876,12 +10876,12 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>GE10/0/5(100M)</t>
+          <t>GE10/0/4(100M)</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/5(100M)</t>
+          <t>IC1.HOR1GE10/0/4(100M)</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -10925,12 +10925,12 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>GE10/0/6(100M)</t>
+          <t>GE10/0/5(100M)</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/6(100M)</t>
+          <t>IC1.HOR1GE10/0/5(100M)</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -10974,12 +10974,12 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>GE10/0/7(100M)</t>
+          <t>GE10/0/6(100M)</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/7(100M)</t>
+          <t>IC1.HOR1GE10/0/6(100M)</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -11023,12 +11023,12 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>GE10/0/8(100M)</t>
+          <t>GE10/0/7(100M)</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/8(100M)</t>
+          <t>IC1.HOR1GE10/0/7(100M)</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -11072,12 +11072,12 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>GE10/0/9(100M)</t>
+          <t>GE10/0/8(100M)</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/9(100M)</t>
+          <t>IC1.HOR1GE10/0/8(100M)</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -11121,12 +11121,12 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>GE10/0/10(100M)</t>
+          <t>GE10/0/9(100M)</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/10(100M)</t>
+          <t>IC1.HOR1GE10/0/9(100M)</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -11170,12 +11170,12 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>GE10/0/11(100M)</t>
+          <t>GE10/0/10(100M)</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/11(100M)</t>
+          <t>IC1.HOR1GE10/0/10(100M)</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -11219,12 +11219,12 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>GE10/0/12(100M)</t>
+          <t>GE10/0/11(100M)</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/12(100M)</t>
+          <t>IC1.HOR1GE10/0/11(100M)</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -11268,12 +11268,12 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>GE10/0/13(100M)</t>
+          <t>GE10/0/12(100M)</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/13(100M)</t>
+          <t>IC1.HOR1GE10/0/12(100M)</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -11317,12 +11317,12 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>GE10/0/14(100M)</t>
+          <t>GE10/0/13(100M)</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/14(100M)</t>
+          <t>IC1.HOR1GE10/0/13(100M)</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -11366,12 +11366,12 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>GE10/0/15(100M)</t>
+          <t>GE10/0/14(100M)</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/15(100M)</t>
+          <t>IC1.HOR1GE10/0/14(100M)</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -11415,12 +11415,12 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>GE10/0/16(100M)</t>
+          <t>GE10/0/15(100M)</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/16(100M)</t>
+          <t>IC1.HOR1GE10/0/15(100M)</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -11464,12 +11464,12 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>GE10/0/17(100M)</t>
+          <t>GE10/0/16(100M)</t>
         </is>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/17(100M)</t>
+          <t>IC1.HOR1GE10/0/16(100M)</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -11513,12 +11513,12 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>GE10/0/18(100M)</t>
+          <t>GE10/0/17(100M)</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/18(100M)</t>
+          <t>IC1.HOR1GE10/0/17(100M)</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -11562,12 +11562,12 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>GE10/0/19(100M)</t>
+          <t>GE10/0/18(100M)</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/19(100M)</t>
+          <t>IC1.HOR1GE10/0/18(100M)</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -11611,12 +11611,12 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>GE10/0/20(100M)</t>
+          <t>GE10/0/19(100M)</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/20(100M)</t>
+          <t>IC1.HOR1GE10/0/19(100M)</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -11660,12 +11660,12 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>GE10/0/21(100M)</t>
+          <t>GE10/0/20(100M)</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/21(100M)</t>
+          <t>IC1.HOR1GE10/0/20(100M)</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -11709,12 +11709,12 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>GE10/0/22(100M)</t>
+          <t>GE10/0/21(100M)</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/22(100M)</t>
+          <t>IC1.HOR1GE10/0/21(100M)</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -11758,12 +11758,12 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>GE10/0/23(100M)</t>
+          <t>GE10/0/22(100M)</t>
         </is>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/23(100M)</t>
+          <t>IC1.HOR1GE10/0/22(100M)</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -11807,12 +11807,12 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>GE10/0/24(100M)</t>
+          <t>GE10/0/23(100M)</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/24(100M)</t>
+          <t>IC1.HOR1GE10/0/23(100M)</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -11856,12 +11856,12 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>GE10/0/25(100M)</t>
+          <t>GE10/0/24(100M)</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/25(100M)</t>
+          <t>IC1.HOR1GE10/0/24(100M)</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -11905,12 +11905,12 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>GE10/0/26(100M)</t>
+          <t>GE10/0/25(100M)</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/26(100M)</t>
+          <t>IC1.HOR1GE10/0/25(100M)</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">

</xml_diff>

<commit_message>
1er version del ansible-runner
</commit_message>
<xml_diff>
--- a/airflow/reports/reporte.xlsx
+++ b/airflow/reports/reporte.xlsx
@@ -547,12 +547,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>100GE2/1/4</t>
+          <t>100GE2/0/0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/4</t>
+          <t>IC1.HOR1100GE2/0/0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/0)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/0)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -600,12 +600,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>100GE9/0/0</t>
+          <t>100GE2/0/1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/0</t>
+          <t>IC1.HOR1100GE2/0/1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -625,14 +625,10 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/2) (32WPU01 2/15/C2) Linea:15008585</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Linea:15008585</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/1)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
           <t>ok</t>
@@ -657,12 +653,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>100GE9/0/1</t>
+          <t>100GE2/0/2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/1</t>
+          <t>IC1.HOR1100GE2/0/2</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -682,14 +678,10 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/3) (32WPU01 2/15/C1) Linea:15008555</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Linea:15008555</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/2)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
           <t>ok</t>
@@ -714,12 +706,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>100GE9/0/2</t>
+          <t>100GE2/0/3</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/2</t>
+          <t>IC1.HOR1100GE2/0/3</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -739,14 +731,10 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/4) (32WPU01 1/14/C1) Linea:15008586</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Linea:15008586</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/3)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
           <t>ok</t>
@@ -771,12 +759,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>100GE9/0/3</t>
+          <t>100GE2/0/4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/3</t>
+          <t>IC1.HOR1100GE2/0/4</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -796,14 +784,10 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/5) (32WPU01 1/16/C1) Linea:15008587</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Linea:15008587</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/4)</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
           <t>ok</t>
@@ -828,12 +812,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>100GE9/0/4</t>
+          <t>100GE2/0/5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/4</t>
+          <t>IC1.HOR1100GE2/0/5</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -853,14 +837,10 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/9/0/6)  (32WPU01 1/16/C2) Linea:15008383</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Linea:15008383</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/5)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>ok</t>
@@ -885,12 +865,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>100GE9/0/5</t>
+          <t>100GE2/0/6</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/5</t>
+          <t>IC1.HOR1100GE2/0/6</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -910,7 +890,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/1) (S004_1 98HOR02 5/1)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/6)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -938,12 +918,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>100GE9/0/6</t>
+          <t>100GE2/0/10</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/6</t>
+          <t>IC1.HOR1100GE2/0/10</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -963,7 +943,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/2) (S004_2 98HOR02 5/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/0)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -991,12 +971,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>100GE9/0/7</t>
+          <t>100GE2/0/11</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/7</t>
+          <t>IC1.HOR1100GE2/0/11</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1016,7 +996,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/0) (S004_3 98HOR02 6/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/1)</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -1044,12 +1024,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>100GE9/0/8</t>
+          <t>100GE2/0/12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/8</t>
+          <t>IC1.HOR1100GE2/0/12</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1069,7 +1049,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/1) (S004_4 98HOR02 6/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/2)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
@@ -1097,12 +1077,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>100GE9/0/9</t>
+          <t>100GE2/0/13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/9</t>
+          <t>IC1.HOR1100GE2/0/13</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1122,7 +1102,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/2) (S004_5 98HOR02 7/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/3)</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -1150,12 +1130,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>100GE9/0/10</t>
+          <t>100GE2/0/14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/10</t>
+          <t>IC1.HOR1100GE2/0/14</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1175,7 +1155,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/2) (S004_6 98HOR02 7/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/0)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -1203,12 +1183,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>100GE9/0/11</t>
+          <t>100GE2/0/15</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/11</t>
+          <t>IC1.HOR1100GE2/0/15</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1228,7 +1208,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/3) (S004_7 98HOR02 8/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/1)</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -1256,12 +1236,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>100GE9/0/12</t>
+          <t>100GE2/0/16</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/12</t>
+          <t>IC1.HOR1100GE2/0/16</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1281,7 +1261,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/4) (WDM3.HOR1 2/3/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/2)</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
@@ -1309,12 +1289,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>100GE9/0/13</t>
+          <t>100GE2/0/17</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/13</t>
+          <t>IC1.HOR1100GE2/0/17</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1334,7 +1314,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/5) (WDM3.HOR1 4/9/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/3)</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -1362,12 +1342,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>100GE9/0/14</t>
+          <t>100GE2/0/18</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/14</t>
+          <t>IC1.HOR1100GE2/0/18</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1387,7 +1367,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/6) (WDM3.HOR1 4/11/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/3/0/3)</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
@@ -1415,12 +1395,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>100GE9/0/15</t>
+          <t>100GE2/0/19</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/15</t>
+          <t>IC1.HOR1100GE2/0/19</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1440,7 +1420,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/3) (WDM3.HOR1 4/1/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/0)</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -1468,12 +1448,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>100GE9/0/16</t>
+          <t>100GE2/1/0</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/16</t>
+          <t>IC1.HOR1100GE2/1/0</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1493,7 +1473,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/4) (WDM3.HOR1 4/3/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/1)</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -1521,12 +1501,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>100GE9/0/17</t>
+          <t>100GE2/1/1</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/17</t>
+          <t>IC1.HOR1100GE2/1/1</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1546,7 +1526,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/5) (WDM3.HOR1 4/4/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/2)</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -1574,12 +1554,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>100GE9/0/18</t>
+          <t>100GE2/1/2</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/18</t>
+          <t>IC1.HOR1100GE2/1/2</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1599,7 +1579,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/8/0/3) (WDM3.HOR1 4/6/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/3)</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
@@ -1627,12 +1607,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>100GE9/0/19</t>
+          <t>100GE2/1/3</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/19</t>
+          <t>IC1.HOR1100GE2/1/3</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1652,7 +1632,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/0/0/11) (WDM3.HOR1 6/8/C2)</t>
+          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/0/0/1)</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -1680,12 +1660,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>100GE9/1/0</t>
+          <t>100GE2/1/4</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/0</t>
+          <t>IC1.HOR1100GE2/1/4</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1705,7 +1685,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/0) (S006_1 98HOR01 1C/6/1)</t>
+          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/0)</t>
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
@@ -1733,12 +1713,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>100GE9/1/1</t>
+          <t>100GE2/1/5</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/1</t>
+          <t>IC1.HOR1100GE2/1/5</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1758,7 +1738,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/1) (S006_2 98HOR01 1C/6/2)</t>
+          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/1)</t>
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
@@ -1786,12 +1766,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>100GE9/1/2</t>
+          <t>100GE8/0/0</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/2</t>
+          <t>IC1.HOR1100GE8/0/0</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1811,7 +1791,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/1/0) (S006_3 98HOR01 1C/7/1)</t>
+          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/0) (S3-005 88HOR02 0/3/1) Linea:11004841</t>
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
@@ -1839,12 +1819,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>100GE9/1/3</t>
+          <t>100GE8/0/1</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/3</t>
+          <t>IC1.HOR1100GE8/0/1</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1864,14 +1844,10 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/0) (S004_8 98HOR02 8/2) Linea:15009213</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Linea:15009213</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/1) (S3-004 88HOR01 0/3/1) Linea:11004840</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
           <t>ok</t>
@@ -1896,12 +1872,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>100GE9/1/4</t>
+          <t>100GE8/0/2</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/4</t>
+          <t>IC1.HOR1100GE8/0/2</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1921,14 +1897,10 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/1) (S004_9 98HOR02 14/1) Linea:15009214</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>Linea:15009214</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/2) (S3-002 88HOR01 0/12/1) Linea:15003692</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
           <t>ok</t>
@@ -1953,12 +1925,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>100GE9/1/5</t>
+          <t>100GE8/0/3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/5</t>
+          <t>IC1.HOR1100GE8/0/3</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1978,14 +1950,10 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/2) (S004_10 98HOR02 14/2) Linea:15009215</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Linea:15009215</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:IRD1NA (Hu0/5/0/0) (S3-001 88HOR02 0/16/1) Linea:15003451</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
           <t>ok</t>
@@ -2010,12 +1978,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>100GE9/1/6</t>
+          <t>100GE9/0/0</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/6</t>
+          <t>IC1.HOR1100GE9/0/0</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2035,12 +2003,12 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/2) (98HOR01 3/1) Linea: 15009094</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/2) (32WPU01 2/15/C2) Linea:15008585</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Linea: 15009094</t>
+          <t>Linea:15008585</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2067,12 +2035,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>100GE9/1/7</t>
+          <t>100GE9/0/1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/7</t>
+          <t>IC1.HOR1100GE9/0/1</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2092,12 +2060,12 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/3) (98HOR01 3/2) Linea: 15009095</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/3) (32WPU01 2/15/C1) Linea:15008555</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Linea: 15009095</t>
+          <t>Linea:15008555</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2124,12 +2092,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>100GE9/1/8</t>
+          <t>100GE9/0/2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/8</t>
+          <t>IC1.HOR1100GE9/0/2</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2149,12 +2117,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/4) (98HOR01 5/1) Linea: 15009096</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/4) (32WPU01 1/14/C1) Linea:15008586</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Linea: 15009096 - BEL1NA</t>
+          <t>Linea:15008586</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2181,12 +2149,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>100GE9/1/9</t>
+          <t>100GE9/0/3</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/9</t>
+          <t>IC1.HOR1100GE9/0/3</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2206,12 +2174,12 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/5) (98HOR01 5/2) Linea: 15009097</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/5) (32WPU01 1/16/C1) Linea:15008587</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Linea: 15009097 - BEL1NA</t>
+          <t>Linea:15008587</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2238,12 +2206,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>100GE9/1/10</t>
+          <t>100GE9/0/4</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/10</t>
+          <t>IC1.HOR1100GE9/0/4</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2263,12 +2231,12 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/6) (98HOR01 4/1) Linea: 15009098</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/9/0/6)  (32WPU01 1/16/C2) Linea:15008383</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Linea: 15009098</t>
+          <t>Linea:15008383</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2295,12 +2263,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>100GE2/0/0</t>
+          <t>100GE9/0/5</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/0</t>
+          <t>IC1.HOR1100GE9/0/5</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2320,7 +2288,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/0)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/1) (S004_1 98HOR02 5/1)</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
@@ -2348,12 +2316,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>100GE2/0/1</t>
+          <t>100GE9/0/6</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/1</t>
+          <t>IC1.HOR1100GE9/0/6</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2373,7 +2341,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/1)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/2) (S004_2 98HOR02 5/2)</t>
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
@@ -2401,12 +2369,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>100GE2/0/2</t>
+          <t>100GE9/0/7</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/2</t>
+          <t>IC1.HOR1100GE9/0/7</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2426,7 +2394,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/2)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/0) (S004_3 98HOR02 6/1)</t>
         </is>
       </c>
       <c r="J36" t="inlineStr"/>
@@ -2454,12 +2422,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>100GE2/0/3</t>
+          <t>100GE9/0/8</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/3</t>
+          <t>IC1.HOR1100GE9/0/8</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2479,7 +2447,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/3)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/1) (S004_4 98HOR02 6/2)</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
@@ -2507,12 +2475,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>100GE2/0/4</t>
+          <t>100GE9/0/9</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/4</t>
+          <t>IC1.HOR1100GE9/0/9</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2532,7 +2500,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/4)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/2) (S004_5 98HOR02 7/1)</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
@@ -2560,12 +2528,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>100GE2/0/5</t>
+          <t>100GE9/0/10</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/5</t>
+          <t>IC1.HOR1100GE9/0/10</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2585,7 +2553,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/5)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/2) (S004_6 98HOR02 7/2)</t>
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
@@ -2613,12 +2581,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>100GE2/0/6</t>
+          <t>100GE9/0/11</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/6</t>
+          <t>IC1.HOR1100GE9/0/11</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2638,7 +2606,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/6)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/3) (S004_7 98HOR02 8/1)</t>
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
@@ -2666,12 +2634,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>100GE2/0/10</t>
+          <t>100GE9/0/12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/10</t>
+          <t>IC1.HOR1100GE9/0/12</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2691,7 +2659,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/0)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/4) (WDM3.HOR1 2/3/C1)</t>
         </is>
       </c>
       <c r="J41" t="inlineStr"/>
@@ -2719,12 +2687,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>100GE2/0/11</t>
+          <t>100GE9/0/13</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/11</t>
+          <t>IC1.HOR1100GE9/0/13</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2744,7 +2712,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/5) (WDM3.HOR1 4/9/C1)</t>
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
@@ -2772,12 +2740,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>100GE2/0/12</t>
+          <t>100GE9/0/14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/12</t>
+          <t>IC1.HOR1100GE9/0/14</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2797,7 +2765,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/2)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/6) (WDM3.HOR1 4/11/C1)</t>
         </is>
       </c>
       <c r="J43" t="inlineStr"/>
@@ -2825,12 +2793,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>100GE2/0/13</t>
+          <t>100GE9/0/15</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/13</t>
+          <t>IC1.HOR1100GE9/0/15</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2850,7 +2818,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/3)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/3) (WDM3.HOR1 4/1/C1)</t>
         </is>
       </c>
       <c r="J44" t="inlineStr"/>
@@ -2878,12 +2846,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>100GE2/0/14</t>
+          <t>100GE9/0/16</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/14</t>
+          <t>IC1.HOR1100GE9/0/16</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2903,7 +2871,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/0)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/4) (WDM3.HOR1 4/3/C1)</t>
         </is>
       </c>
       <c r="J45" t="inlineStr"/>
@@ -2931,12 +2899,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>100GE2/0/15</t>
+          <t>100GE9/0/17</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/15</t>
+          <t>IC1.HOR1100GE9/0/17</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2956,7 +2924,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/5) (WDM3.HOR1 4/4/C1)</t>
         </is>
       </c>
       <c r="J46" t="inlineStr"/>
@@ -2984,12 +2952,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>100GE2/0/16</t>
+          <t>100GE9/0/18</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/16</t>
+          <t>IC1.HOR1100GE9/0/18</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3009,7 +2977,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/2)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/8/0/3) (WDM3.HOR1 4/6/C1)</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -3037,12 +3005,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>100GE2/0/17</t>
+          <t>100GE9/0/19</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/17</t>
+          <t>IC1.HOR1100GE9/0/19</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3062,7 +3030,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/3)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/0/0/11) (WDM3.HOR1 6/8/C2)</t>
         </is>
       </c>
       <c r="J48" t="inlineStr"/>
@@ -3090,12 +3058,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>100GE2/0/18</t>
+          <t>100GE9/1/0</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/18</t>
+          <t>IC1.HOR1100GE9/1/0</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -3115,7 +3083,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/3/0/3)</t>
+          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/0) (S006_1 98HOR01 1C/6/1)</t>
         </is>
       </c>
       <c r="J49" t="inlineStr"/>
@@ -3143,12 +3111,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>100GE2/0/19</t>
+          <t>100GE9/1/1</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/19</t>
+          <t>IC1.HOR1100GE9/1/1</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3168,7 +3136,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/0)</t>
+          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/1) (S006_2 98HOR01 1C/6/2)</t>
         </is>
       </c>
       <c r="J50" t="inlineStr"/>
@@ -3196,12 +3164,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>100GE2/1/0</t>
+          <t>100GE9/1/2</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/0</t>
+          <t>IC1.HOR1100GE9/1/2</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -3221,7 +3189,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/1)</t>
+          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/1/0) (S006_3 98HOR01 1C/7/1)</t>
         </is>
       </c>
       <c r="J51" t="inlineStr"/>
@@ -3249,12 +3217,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>100GE2/1/1</t>
+          <t>100GE9/1/3</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/1</t>
+          <t>IC1.HOR1100GE9/1/3</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -3274,10 +3242,14 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/2)</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr"/>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/0) (S004_8 98HOR02 8/2) Linea:15009213</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Linea:15009213</t>
+        </is>
+      </c>
       <c r="K52" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3302,12 +3274,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>100GE2/1/2</t>
+          <t>100GE9/1/4</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/2</t>
+          <t>IC1.HOR1100GE9/1/4</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -3327,10 +3299,14 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/3)</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr"/>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/1) (S004_9 98HOR02 14/1) Linea:15009214</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Linea:15009214</t>
+        </is>
+      </c>
       <c r="K53" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3355,12 +3331,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>100GE2/1/3</t>
+          <t>100GE9/1/5</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/3</t>
+          <t>IC1.HOR1100GE9/1/5</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -3380,10 +3356,14 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/0/0/1)</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr"/>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/2) (S004_10 98HOR02 14/2) Linea:15009215</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Linea:15009215</t>
+        </is>
+      </c>
       <c r="K54" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3408,12 +3388,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>100GE2/1/5</t>
+          <t>100GE9/1/6</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/5</t>
+          <t>IC1.HOR1100GE9/1/6</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -3433,10 +3413,14 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/1)</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/2) (98HOR01 3/1) Linea: 15009094</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Linea: 15009094</t>
+        </is>
+      </c>
       <c r="K55" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3461,12 +3445,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>100GE8/0/0</t>
+          <t>100GE9/1/7</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/0</t>
+          <t>IC1.HOR1100GE9/1/7</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -3486,10 +3470,14 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/0) (S3-005 88HOR02 0/3/1) Linea:11004841</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/3) (98HOR01 3/2) Linea: 15009095</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Linea: 15009095</t>
+        </is>
+      </c>
       <c r="K56" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3514,12 +3502,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>100GE8/0/1</t>
+          <t>100GE9/1/8</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/1</t>
+          <t>IC1.HOR1100GE9/1/8</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -3539,10 +3527,14 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/1) (S3-004 88HOR01 0/3/1) Linea:11004840</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/4) (98HOR01 5/1) Linea: 15009096</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Linea: 15009096 - BEL1NA</t>
+        </is>
+      </c>
       <c r="K57" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3567,12 +3559,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>100GE8/0/2</t>
+          <t>100GE9/1/9</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/2</t>
+          <t>IC1.HOR1100GE9/1/9</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -3592,10 +3584,14 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/2) (S3-002 88HOR01 0/12/1) Linea:15003692</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/5) (98HOR01 5/2) Linea: 15009097</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Linea: 15009097 - BEL1NA</t>
+        </is>
+      </c>
       <c r="K58" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3620,12 +3616,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>100GE8/0/3</t>
+          <t>100GE9/1/10</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/3</t>
+          <t>IC1.HOR1100GE9/1/10</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -3645,10 +3641,14 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/5/0/0) (S3-001 88HOR02 0/16/1) Linea:15003451</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/6) (98HOR01 4/1) Linea: 15009098</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Linea: 15009098</t>
+        </is>
+      </c>
       <c r="K59" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3673,17 +3673,17 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>100GE8/1/7</t>
+          <t>GE10/0/26(100M)</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/7</t>
+          <t>IC1.HOR1GE10/0/26(100M)</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>100GE</t>
+          <t>GE</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -3722,12 +3722,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>100GE8/1/8</t>
+          <t>100GE2/0/8</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/8</t>
+          <t>IC1.HOR1100GE2/0/8</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -3771,12 +3771,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>100GE8/1/9</t>
+          <t>100GE2/0/9</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/9</t>
+          <t>IC1.HOR1100GE2/0/9</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -3820,12 +3820,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>100GE8/1/10</t>
+          <t>100GE2/1/6</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/10</t>
+          <t>IC1.HOR1100GE2/1/6</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3869,12 +3869,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>100GE8/1/11</t>
+          <t>100GE2/1/14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/11</t>
+          <t>IC1.HOR1100GE2/1/14</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3918,12 +3918,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>100GE8/1/12</t>
+          <t>100GE2/1/15</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/12</t>
+          <t>IC1.HOR1100GE2/1/15</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3967,12 +3967,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>100GE8/1/13</t>
+          <t>100GE2/1/16</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/13</t>
+          <t>IC1.HOR1100GE2/1/16</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -4016,12 +4016,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>100GE8/1/14</t>
+          <t>100GE2/1/17</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/14</t>
+          <t>IC1.HOR1100GE2/1/17</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -4065,12 +4065,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>100GE8/1/15</t>
+          <t>100GE2/1/18</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/15</t>
+          <t>IC1.HOR1100GE2/1/18</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -4114,12 +4114,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>100GE8/1/16</t>
+          <t>100GE2/1/19</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/16</t>
+          <t>IC1.HOR1100GE2/1/19</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -4163,12 +4163,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>100GE8/1/17</t>
+          <t>100GE3/0/7</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/17</t>
+          <t>IC1.HOR1100GE3/0/7</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -4212,12 +4212,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>100GE8/1/18</t>
+          <t>100GE3/0/8</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/18</t>
+          <t>IC1.HOR1100GE3/0/8</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -4261,12 +4261,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>100GE8/1/19</t>
+          <t>100GE3/0/9</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/19</t>
+          <t>IC1.HOR1100GE3/0/9</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -4310,12 +4310,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>100GE9/1/11</t>
+          <t>100GE3/0/10</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/11</t>
+          <t>IC1.HOR1100GE3/0/10</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -4359,12 +4359,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>100GE9/1/12</t>
+          <t>100GE3/0/11</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/12</t>
+          <t>IC1.HOR1100GE3/0/11</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -4408,12 +4408,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>100GE9/1/13</t>
+          <t>100GE3/0/12</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/13</t>
+          <t>IC1.HOR1100GE3/0/12</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -4457,12 +4457,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>100GE9/1/14</t>
+          <t>100GE3/0/13</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/14</t>
+          <t>IC1.HOR1100GE3/0/13</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -4506,12 +4506,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>100GE9/1/15</t>
+          <t>100GE3/0/14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/15</t>
+          <t>IC1.HOR1100GE3/0/14</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -4555,12 +4555,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>100GE9/1/16</t>
+          <t>100GE3/0/15</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/16</t>
+          <t>IC1.HOR1100GE3/0/15</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -4604,12 +4604,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>100GE9/1/17</t>
+          <t>100GE3/0/16</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/17</t>
+          <t>IC1.HOR1100GE3/0/16</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -4653,12 +4653,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>100GE9/1/18</t>
+          <t>100GE3/0/17</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/18</t>
+          <t>IC1.HOR1100GE3/0/17</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -4702,12 +4702,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>100GE9/1/19</t>
+          <t>100GE3/0/18</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/19</t>
+          <t>IC1.HOR1100GE3/0/18</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -4751,12 +4751,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>100GE2/0/8</t>
+          <t>100GE3/0/19</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/8</t>
+          <t>IC1.HOR1100GE3/0/19</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -4800,12 +4800,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>100GE2/0/9</t>
+          <t>100GE3/1/0</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/9</t>
+          <t>IC1.HOR1100GE3/1/0</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -4849,17 +4849,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>GE10/0/26(100M)</t>
+          <t>100GE3/1/1</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/26(100M)</t>
+          <t>IC1.HOR1100GE3/1/1</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>100GE</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -4898,12 +4898,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>100GE2/1/6</t>
+          <t>100GE3/1/2</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/6</t>
+          <t>IC1.HOR1100GE3/1/2</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -4947,12 +4947,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>100GE2/1/14</t>
+          <t>100GE3/1/3</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/14</t>
+          <t>IC1.HOR1100GE3/1/3</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -4996,12 +4996,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>100GE2/1/15</t>
+          <t>100GE3/1/4</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/15</t>
+          <t>IC1.HOR1100GE3/1/4</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -5045,12 +5045,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>100GE2/1/16</t>
+          <t>100GE3/1/5</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/16</t>
+          <t>IC1.HOR1100GE3/1/5</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -5094,12 +5094,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>100GE2/1/17</t>
+          <t>100GE3/1/6</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/17</t>
+          <t>IC1.HOR1100GE3/1/6</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -5143,12 +5143,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>100GE2/1/18</t>
+          <t>100GE3/1/7</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/18</t>
+          <t>IC1.HOR1100GE3/1/7</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -5192,12 +5192,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>100GE2/1/19</t>
+          <t>100GE3/1/8</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/19</t>
+          <t>IC1.HOR1100GE3/1/8</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -5241,12 +5241,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>100GE3/0/7</t>
+          <t>100GE3/1/9</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/7</t>
+          <t>IC1.HOR1100GE3/1/9</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -5290,12 +5290,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>100GE3/0/8</t>
+          <t>100GE3/1/10</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/8</t>
+          <t>IC1.HOR1100GE3/1/10</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -5339,12 +5339,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>100GE3/0/9</t>
+          <t>100GE3/1/11</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/9</t>
+          <t>IC1.HOR1100GE3/1/11</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -5388,12 +5388,12 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>100GE3/0/10</t>
+          <t>100GE3/1/12</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/10</t>
+          <t>IC1.HOR1100GE3/1/12</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -5437,12 +5437,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>100GE3/0/11</t>
+          <t>100GE3/1/13</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/11</t>
+          <t>IC1.HOR1100GE3/1/13</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -5486,12 +5486,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>100GE3/0/12</t>
+          <t>100GE3/1/14</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/12</t>
+          <t>IC1.HOR1100GE3/1/14</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -5535,12 +5535,12 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>100GE3/0/13</t>
+          <t>100GE3/1/15</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/13</t>
+          <t>IC1.HOR1100GE3/1/15</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -5584,12 +5584,12 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>100GE3/0/14</t>
+          <t>100GE3/1/16</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/14</t>
+          <t>IC1.HOR1100GE3/1/16</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -5633,12 +5633,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>100GE3/0/15</t>
+          <t>100GE3/1/17</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/15</t>
+          <t>IC1.HOR1100GE3/1/17</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -5682,12 +5682,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>100GE3/0/16</t>
+          <t>100GE3/1/18</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/16</t>
+          <t>IC1.HOR1100GE3/1/18</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -5731,12 +5731,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>100GE3/0/17</t>
+          <t>100GE3/1/19</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/17</t>
+          <t>IC1.HOR1100GE3/1/19</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -5780,17 +5780,17 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>100GE3/0/18</t>
+          <t>GE10/0/27(100M)</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/18</t>
+          <t>IC1.HOR1GE10/0/27(100M)</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>100GE</t>
+          <t>GE</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -5829,12 +5829,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>100GE3/0/19</t>
+          <t>100GE8/0/9</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/0/19</t>
+          <t>IC1.HOR1100GE8/0/9</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -5878,12 +5878,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>100GE3/1/0</t>
+          <t>100GE8/0/10</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/0</t>
+          <t>IC1.HOR1100GE8/0/10</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -5927,12 +5927,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>100GE3/1/1</t>
+          <t>100GE8/0/11</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/1</t>
+          <t>IC1.HOR1100GE8/0/11</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -5976,12 +5976,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>100GE3/1/2</t>
+          <t>100GE8/0/12</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/2</t>
+          <t>IC1.HOR1100GE8/0/12</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -6025,12 +6025,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>100GE3/1/3</t>
+          <t>100GE8/0/13</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/3</t>
+          <t>IC1.HOR1100GE8/0/13</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -6074,12 +6074,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>100GE3/1/4</t>
+          <t>100GE8/0/14</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/4</t>
+          <t>IC1.HOR1100GE8/0/14</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -6123,12 +6123,12 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>100GE3/1/5</t>
+          <t>100GE8/0/15</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/5</t>
+          <t>IC1.HOR1100GE8/0/15</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -6172,12 +6172,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>100GE3/1/6</t>
+          <t>100GE8/0/16</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/6</t>
+          <t>IC1.HOR1100GE8/0/16</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -6221,12 +6221,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>100GE3/1/7</t>
+          <t>100GE8/0/17</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/7</t>
+          <t>IC1.HOR1100GE8/0/17</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -6270,12 +6270,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>100GE3/1/8</t>
+          <t>100GE8/0/18</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/8</t>
+          <t>IC1.HOR1100GE8/0/18</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -6319,12 +6319,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>100GE3/1/9</t>
+          <t>100GE8/0/19</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/9</t>
+          <t>IC1.HOR1100GE8/0/19</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -6368,12 +6368,12 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>100GE3/1/10</t>
+          <t>100GE8/1/0</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/10</t>
+          <t>IC1.HOR1100GE8/1/0</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -6417,12 +6417,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>100GE3/1/11</t>
+          <t>100GE8/1/1</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/11</t>
+          <t>IC1.HOR1100GE8/1/1</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -6466,12 +6466,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>100GE3/1/12</t>
+          <t>100GE8/1/2</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/12</t>
+          <t>IC1.HOR1100GE8/1/2</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -6515,12 +6515,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>100GE3/1/13</t>
+          <t>100GE8/1/3</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/13</t>
+          <t>IC1.HOR1100GE8/1/3</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -6564,12 +6564,12 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>100GE3/1/14</t>
+          <t>100GE8/1/4</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/14</t>
+          <t>IC1.HOR1100GE8/1/4</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -6613,12 +6613,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>100GE3/1/15</t>
+          <t>100GE8/1/5</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/15</t>
+          <t>IC1.HOR1100GE8/1/5</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -6662,12 +6662,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>100GE3/1/16</t>
+          <t>100GE8/1/6</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/16</t>
+          <t>IC1.HOR1100GE8/1/6</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -6711,12 +6711,12 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>100GE3/1/17</t>
+          <t>100GE8/1/7</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/17</t>
+          <t>IC1.HOR1100GE8/1/7</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -6760,12 +6760,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>100GE3/1/18</t>
+          <t>100GE8/1/8</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/18</t>
+          <t>IC1.HOR1100GE8/1/8</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -6809,12 +6809,12 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>100GE3/1/19</t>
+          <t>100GE8/1/9</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE3/1/19</t>
+          <t>IC1.HOR1100GE8/1/9</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -6858,12 +6858,12 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>100GE8/0/9</t>
+          <t>100GE8/1/10</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/9</t>
+          <t>IC1.HOR1100GE8/1/10</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -6907,12 +6907,12 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>100GE8/0/10</t>
+          <t>100GE8/1/11</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/10</t>
+          <t>IC1.HOR1100GE8/1/11</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -6956,12 +6956,12 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>100GE8/0/11</t>
+          <t>100GE8/1/12</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/11</t>
+          <t>IC1.HOR1100GE8/1/12</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -7005,12 +7005,12 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>100GE8/0/12</t>
+          <t>100GE8/1/13</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/12</t>
+          <t>IC1.HOR1100GE8/1/13</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -7054,12 +7054,12 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>100GE8/0/13</t>
+          <t>100GE8/1/14</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/13</t>
+          <t>IC1.HOR1100GE8/1/14</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -7103,12 +7103,12 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>100GE8/0/14</t>
+          <t>100GE8/1/15</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/14</t>
+          <t>IC1.HOR1100GE8/1/15</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -7152,12 +7152,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>100GE8/0/15</t>
+          <t>100GE8/1/16</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/15</t>
+          <t>IC1.HOR1100GE8/1/16</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -7201,12 +7201,12 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>100GE8/0/16</t>
+          <t>100GE8/1/17</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/16</t>
+          <t>IC1.HOR1100GE8/1/17</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -7250,12 +7250,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>100GE8/0/17</t>
+          <t>100GE8/1/18</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/17</t>
+          <t>IC1.HOR1100GE8/1/18</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -7299,12 +7299,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>100GE8/0/18</t>
+          <t>100GE8/1/19</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/18</t>
+          <t>IC1.HOR1100GE8/1/19</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -7348,12 +7348,12 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>100GE8/0/19</t>
+          <t>100GE9/1/11</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/19</t>
+          <t>IC1.HOR1100GE9/1/11</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -7397,12 +7397,12 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>100GE8/1/0</t>
+          <t>100GE9/1/12</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/0</t>
+          <t>IC1.HOR1100GE9/1/12</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -7446,12 +7446,12 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>100GE8/1/1</t>
+          <t>100GE9/1/13</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/1</t>
+          <t>IC1.HOR1100GE9/1/13</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -7495,12 +7495,12 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>100GE8/1/2</t>
+          <t>100GE9/1/14</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/2</t>
+          <t>IC1.HOR1100GE9/1/14</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -7544,12 +7544,12 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>100GE8/1/3</t>
+          <t>100GE9/1/15</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/3</t>
+          <t>IC1.HOR1100GE9/1/15</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -7593,12 +7593,12 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>100GE8/1/4</t>
+          <t>100GE9/1/16</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/4</t>
+          <t>IC1.HOR1100GE9/1/16</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -7642,12 +7642,12 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>100GE8/1/5</t>
+          <t>100GE9/1/17</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/5</t>
+          <t>IC1.HOR1100GE9/1/17</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -7691,12 +7691,12 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>100GE8/1/6</t>
+          <t>100GE9/1/18</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/1/6</t>
+          <t>IC1.HOR1100GE9/1/18</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -7740,17 +7740,17 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>GE1/0/0(100M)</t>
+          <t>100GE9/1/19</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/0(100M)</t>
+          <t>IC1.HOR1100GE9/1/19</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>100GE</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
@@ -7789,12 +7789,12 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>GE1/0/1(100M)</t>
+          <t>GE1/0/0(100M)</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/1(100M)</t>
+          <t>IC1.HOR1GE1/0/0(100M)</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -7838,12 +7838,12 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>GE1/0/2(100M)</t>
+          <t>GE1/0/1(100M)</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/2(100M)</t>
+          <t>IC1.HOR1GE1/0/1(100M)</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -7887,12 +7887,12 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>GE1/0/3(100M)</t>
+          <t>GE1/0/2(100M)</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/3(100M)</t>
+          <t>IC1.HOR1GE1/0/2(100M)</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -7936,12 +7936,12 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>GE1/0/4(100M)</t>
+          <t>GE1/0/3(100M)</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/4(100M)</t>
+          <t>IC1.HOR1GE1/0/3(100M)</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -7985,12 +7985,12 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>GE1/0/5(100M)</t>
+          <t>GE1/0/4(100M)</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/5(100M)</t>
+          <t>IC1.HOR1GE1/0/4(100M)</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -8034,12 +8034,12 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>GE1/0/6(100M)</t>
+          <t>GE1/0/5(100M)</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/6(100M)</t>
+          <t>IC1.HOR1GE1/0/5(100M)</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -8083,12 +8083,12 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>GE1/0/7(100M)</t>
+          <t>GE1/0/6(100M)</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/7(100M)</t>
+          <t>IC1.HOR1GE1/0/6(100M)</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -8132,12 +8132,12 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>GE1/0/8(100M)</t>
+          <t>GE1/0/7(100M)</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/8(100M)</t>
+          <t>IC1.HOR1GE1/0/7(100M)</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -8181,12 +8181,12 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>GE1/0/9(100M)</t>
+          <t>GE1/0/8(100M)</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/9(100M)</t>
+          <t>IC1.HOR1GE1/0/8(100M)</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -8230,12 +8230,12 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>GE1/0/10(100M)</t>
+          <t>GE1/0/9(100M)</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/10(100M)</t>
+          <t>IC1.HOR1GE1/0/9(100M)</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -8279,12 +8279,12 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>GE1/0/11(100M)</t>
+          <t>GE1/0/10(100M)</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/11(100M)</t>
+          <t>IC1.HOR1GE1/0/10(100M)</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -8328,12 +8328,12 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>GE1/0/12(100M)</t>
+          <t>GE1/0/11(100M)</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/12(100M)</t>
+          <t>IC1.HOR1GE1/0/11(100M)</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -8377,12 +8377,12 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>GE1/0/13(100M)</t>
+          <t>GE1/0/12(100M)</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/13(100M)</t>
+          <t>IC1.HOR1GE1/0/12(100M)</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -8426,12 +8426,12 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>GE1/0/14(100M)</t>
+          <t>GE1/0/13(100M)</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/14(100M)</t>
+          <t>IC1.HOR1GE1/0/13(100M)</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -8475,12 +8475,12 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>GE1/0/15(100M)</t>
+          <t>GE1/0/14(100M)</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/15(100M)</t>
+          <t>IC1.HOR1GE1/0/14(100M)</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -8524,12 +8524,12 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>GE1/0/16(100M)</t>
+          <t>GE1/0/15(100M)</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/16(100M)</t>
+          <t>IC1.HOR1GE1/0/15(100M)</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -8573,12 +8573,12 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>GE1/0/17(100M)</t>
+          <t>GE1/0/16(100M)</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/17(100M)</t>
+          <t>IC1.HOR1GE1/0/16(100M)</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -8622,12 +8622,12 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>GE1/0/18(100M)</t>
+          <t>GE1/0/17(100M)</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/18(100M)</t>
+          <t>IC1.HOR1GE1/0/17(100M)</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -8671,12 +8671,12 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>GE1/0/19(100M)</t>
+          <t>GE1/0/18(100M)</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/19(100M)</t>
+          <t>IC1.HOR1GE1/0/18(100M)</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -8720,12 +8720,12 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>GE1/0/20(100M)</t>
+          <t>GE1/0/19(100M)</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/20(100M)</t>
+          <t>IC1.HOR1GE1/0/19(100M)</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -8769,12 +8769,12 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>GE1/0/21(100M)</t>
+          <t>GE1/0/20(100M)</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/21(100M)</t>
+          <t>IC1.HOR1GE1/0/20(100M)</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -8818,12 +8818,12 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>GE1/0/22(100M)</t>
+          <t>GE1/0/21(100M)</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/22(100M)</t>
+          <t>IC1.HOR1GE1/0/21(100M)</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -8867,12 +8867,12 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>GE1/0/23(100M)</t>
+          <t>GE1/0/22(100M)</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/23(100M)</t>
+          <t>IC1.HOR1GE1/0/22(100M)</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -8916,12 +8916,12 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>GE1/0/24(100M)</t>
+          <t>GE1/0/23(100M)</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/24(100M)</t>
+          <t>IC1.HOR1GE1/0/23(100M)</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -8965,12 +8965,12 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>GE1/0/25(100M)</t>
+          <t>GE1/0/24(100M)</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/25(100M)</t>
+          <t>IC1.HOR1GE1/0/24(100M)</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -9014,12 +9014,12 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>GE1/0/26(100M)</t>
+          <t>GE1/0/25(100M)</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/26(100M)</t>
+          <t>IC1.HOR1GE1/0/25(100M)</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -9063,12 +9063,12 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>GE1/0/27(100M)</t>
+          <t>GE1/0/26(100M)</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/27(100M)</t>
+          <t>IC1.HOR1GE1/0/26(100M)</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -9112,12 +9112,12 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>GE1/0/28(100M)</t>
+          <t>GE1/0/27(100M)</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/28(100M)</t>
+          <t>IC1.HOR1GE1/0/27(100M)</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -9161,12 +9161,12 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>GE1/0/29(100M)</t>
+          <t>GE1/0/28(100M)</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/29(100M)</t>
+          <t>IC1.HOR1GE1/0/28(100M)</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -9210,12 +9210,12 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>GE1/0/30(100M)</t>
+          <t>GE1/0/29(100M)</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/30(100M)</t>
+          <t>IC1.HOR1GE1/0/29(100M)</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -9259,12 +9259,12 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>GE1/0/31(100M)</t>
+          <t>GE1/0/30(100M)</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/31(100M)</t>
+          <t>IC1.HOR1GE1/0/30(100M)</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -9308,12 +9308,12 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>GE1/0/32(100M)</t>
+          <t>GE1/0/31(100M)</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/32(100M)</t>
+          <t>IC1.HOR1GE1/0/31(100M)</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -9357,12 +9357,12 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>GE1/0/33(100M)</t>
+          <t>GE1/0/32(100M)</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/33(100M)</t>
+          <t>IC1.HOR1GE1/0/32(100M)</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -9406,12 +9406,12 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>GE1/0/34(100M)</t>
+          <t>GE1/0/33(100M)</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/34(100M)</t>
+          <t>IC1.HOR1GE1/0/33(100M)</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -9455,12 +9455,12 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>GE1/0/35(100M)</t>
+          <t>GE1/0/34(100M)</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/35(100M)</t>
+          <t>IC1.HOR1GE1/0/34(100M)</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -9504,12 +9504,12 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>GE1/0/36(100M)</t>
+          <t>GE1/0/35(100M)</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/36(100M)</t>
+          <t>IC1.HOR1GE1/0/35(100M)</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -9553,12 +9553,12 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>GE1/0/37(100M)</t>
+          <t>GE1/0/36(100M)</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/37(100M)</t>
+          <t>IC1.HOR1GE1/0/36(100M)</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -9602,12 +9602,12 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>GE1/0/38(100M)</t>
+          <t>GE1/0/37(100M)</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/38(100M)</t>
+          <t>IC1.HOR1GE1/0/37(100M)</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -9651,12 +9651,12 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>GE1/0/39(100M)</t>
+          <t>GE1/0/38(100M)</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/39(100M)</t>
+          <t>IC1.HOR1GE1/0/38(100M)</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -9700,12 +9700,12 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>GE1/0/40(100M)</t>
+          <t>GE1/0/39(100M)</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/40(100M)</t>
+          <t>IC1.HOR1GE1/0/39(100M)</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -9749,12 +9749,12 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>GE1/0/41(100M)</t>
+          <t>GE1/0/40(100M)</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/41(100M)</t>
+          <t>IC1.HOR1GE1/0/40(100M)</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -9798,12 +9798,12 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>GE1/0/42(100M)</t>
+          <t>GE1/0/41(100M)</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/42(100M)</t>
+          <t>IC1.HOR1GE1/0/41(100M)</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -9847,12 +9847,12 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>GE1/0/43(100M)</t>
+          <t>GE1/0/42(100M)</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/43(100M)</t>
+          <t>IC1.HOR1GE1/0/42(100M)</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -9896,12 +9896,12 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>GE1/0/44(100M)</t>
+          <t>GE1/0/43(100M)</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/44(100M)</t>
+          <t>IC1.HOR1GE1/0/43(100M)</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -9945,12 +9945,12 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>GE1/0/45(100M)</t>
+          <t>GE1/0/44(100M)</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/45(100M)</t>
+          <t>IC1.HOR1GE1/0/44(100M)</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -9994,12 +9994,12 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>GE1/0/46(100M)</t>
+          <t>GE1/0/45(100M)</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/46(100M)</t>
+          <t>IC1.HOR1GE1/0/45(100M)</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -10043,12 +10043,12 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>GE1/0/47(100M)</t>
+          <t>GE1/0/46(100M)</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/47(100M)</t>
+          <t>IC1.HOR1GE1/0/46(100M)</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -10092,12 +10092,12 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>GE1/0/48(100M)</t>
+          <t>GE1/0/47(100M)</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/48(100M)</t>
+          <t>IC1.HOR1GE1/0/47(100M)</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -10141,12 +10141,12 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>GE1/0/49(100M)</t>
+          <t>GE1/0/48(100M)</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/49(100M)</t>
+          <t>IC1.HOR1GE1/0/48(100M)</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -10190,12 +10190,12 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>GE1/0/50(100M)</t>
+          <t>GE1/0/49(100M)</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/50(100M)</t>
+          <t>IC1.HOR1GE1/0/49(100M)</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -10239,12 +10239,12 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>GE1/0/51(100M)</t>
+          <t>GE1/0/50(100M)</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/51(100M)</t>
+          <t>IC1.HOR1GE1/0/50(100M)</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -10288,12 +10288,12 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>GE1/0/52(100M)</t>
+          <t>GE1/0/51(100M)</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/52(100M)</t>
+          <t>IC1.HOR1GE1/0/51(100M)</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -10337,12 +10337,12 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>GE1/0/53(100M)</t>
+          <t>GE1/0/52(100M)</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/53(100M)</t>
+          <t>IC1.HOR1GE1/0/52(100M)</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -10386,12 +10386,12 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>GE1/0/54(100M)</t>
+          <t>GE1/0/53(100M)</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/54(100M)</t>
+          <t>IC1.HOR1GE1/0/53(100M)</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -10435,12 +10435,12 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>GE1/0/55(100M)</t>
+          <t>GE1/0/54(100M)</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/55(100M)</t>
+          <t>IC1.HOR1GE1/0/54(100M)</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -10484,12 +10484,12 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>GE1/0/56(100M)</t>
+          <t>GE1/0/55(100M)</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/56(100M)</t>
+          <t>IC1.HOR1GE1/0/55(100M)</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -10533,12 +10533,12 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>GE1/0/57(100M)</t>
+          <t>GE1/0/56(100M)</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/57(100M)</t>
+          <t>IC1.HOR1GE1/0/56(100M)</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -10582,12 +10582,12 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>GE1/0/58(100M)</t>
+          <t>GE1/0/57(100M)</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/58(100M)</t>
+          <t>IC1.HOR1GE1/0/57(100M)</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -10631,12 +10631,12 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>GE1/0/59(100M)</t>
+          <t>GE1/0/58(100M)</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE1/0/59(100M)</t>
+          <t>IC1.HOR1GE1/0/58(100M)</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -10680,12 +10680,12 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>GE10/0/0(100M)</t>
+          <t>GE1/0/59(100M)</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/0(100M)</t>
+          <t>IC1.HOR1GE1/0/59(100M)</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -10729,12 +10729,12 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>GE10/0/1(100M)</t>
+          <t>GE10/0/0(100M)</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/1(100M)</t>
+          <t>IC1.HOR1GE10/0/0(100M)</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -10778,12 +10778,12 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>GE10/0/2(100M)</t>
+          <t>GE10/0/1(100M)</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/2(100M)</t>
+          <t>IC1.HOR1GE10/0/1(100M)</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -10827,12 +10827,12 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>GE10/0/3(100M)</t>
+          <t>GE10/0/2(100M)</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/3(100M)</t>
+          <t>IC1.HOR1GE10/0/2(100M)</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -10876,12 +10876,12 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>GE10/0/4(100M)</t>
+          <t>GE10/0/3(100M)</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/4(100M)</t>
+          <t>IC1.HOR1GE10/0/3(100M)</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -10925,12 +10925,12 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>GE10/0/5(100M)</t>
+          <t>GE10/0/4(100M)</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/5(100M)</t>
+          <t>IC1.HOR1GE10/0/4(100M)</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -10974,12 +10974,12 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>GE10/0/6(100M)</t>
+          <t>GE10/0/5(100M)</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/6(100M)</t>
+          <t>IC1.HOR1GE10/0/5(100M)</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -11023,12 +11023,12 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>GE10/0/7(100M)</t>
+          <t>GE10/0/6(100M)</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/7(100M)</t>
+          <t>IC1.HOR1GE10/0/6(100M)</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -11072,12 +11072,12 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>GE10/0/8(100M)</t>
+          <t>GE10/0/7(100M)</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/8(100M)</t>
+          <t>IC1.HOR1GE10/0/7(100M)</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -11121,12 +11121,12 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>GE10/0/9(100M)</t>
+          <t>GE10/0/8(100M)</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/9(100M)</t>
+          <t>IC1.HOR1GE10/0/8(100M)</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -11170,12 +11170,12 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>GE10/0/10(100M)</t>
+          <t>GE10/0/9(100M)</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/10(100M)</t>
+          <t>IC1.HOR1GE10/0/9(100M)</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -11219,12 +11219,12 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>GE10/0/11(100M)</t>
+          <t>GE10/0/10(100M)</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/11(100M)</t>
+          <t>IC1.HOR1GE10/0/10(100M)</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -11268,12 +11268,12 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>GE10/0/12(100M)</t>
+          <t>GE10/0/11(100M)</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/12(100M)</t>
+          <t>IC1.HOR1GE10/0/11(100M)</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -11317,12 +11317,12 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>GE10/0/13(100M)</t>
+          <t>GE10/0/12(100M)</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/13(100M)</t>
+          <t>IC1.HOR1GE10/0/12(100M)</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -11366,12 +11366,12 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>GE10/0/14(100M)</t>
+          <t>GE10/0/13(100M)</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/14(100M)</t>
+          <t>IC1.HOR1GE10/0/13(100M)</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -11415,12 +11415,12 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>GE10/0/15(100M)</t>
+          <t>GE10/0/14(100M)</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/15(100M)</t>
+          <t>IC1.HOR1GE10/0/14(100M)</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -11464,12 +11464,12 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>GE10/0/16(100M)</t>
+          <t>GE10/0/15(100M)</t>
         </is>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/16(100M)</t>
+          <t>IC1.HOR1GE10/0/15(100M)</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -11513,12 +11513,12 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>GE10/0/17(100M)</t>
+          <t>GE10/0/16(100M)</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/17(100M)</t>
+          <t>IC1.HOR1GE10/0/16(100M)</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -11562,12 +11562,12 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>GE10/0/18(100M)</t>
+          <t>GE10/0/17(100M)</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/18(100M)</t>
+          <t>IC1.HOR1GE10/0/17(100M)</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -11611,12 +11611,12 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>GE10/0/19(100M)</t>
+          <t>GE10/0/18(100M)</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/19(100M)</t>
+          <t>IC1.HOR1GE10/0/18(100M)</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -11660,12 +11660,12 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>GE10/0/20(100M)</t>
+          <t>GE10/0/19(100M)</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/20(100M)</t>
+          <t>IC1.HOR1GE10/0/19(100M)</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -11709,12 +11709,12 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>GE10/0/21(100M)</t>
+          <t>GE10/0/20(100M)</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/21(100M)</t>
+          <t>IC1.HOR1GE10/0/20(100M)</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -11758,12 +11758,12 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>GE10/0/22(100M)</t>
+          <t>GE10/0/21(100M)</t>
         </is>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/22(100M)</t>
+          <t>IC1.HOR1GE10/0/21(100M)</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -11807,12 +11807,12 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>GE10/0/23(100M)</t>
+          <t>GE10/0/22(100M)</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/23(100M)</t>
+          <t>IC1.HOR1GE10/0/22(100M)</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -11856,12 +11856,12 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>GE10/0/24(100M)</t>
+          <t>GE10/0/23(100M)</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/24(100M)</t>
+          <t>IC1.HOR1GE10/0/23(100M)</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -11905,12 +11905,12 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>GE10/0/25(100M)</t>
+          <t>GE10/0/24(100M)</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/25(100M)</t>
+          <t>IC1.HOR1GE10/0/24(100M)</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -11954,12 +11954,12 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>GE10/0/27(100M)</t>
+          <t>GE10/0/25(100M)</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>IC1.HOR1GE10/0/27(100M)</t>
+          <t>IC1.HOR1GE10/0/25(100M)</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">

</xml_diff>

<commit_message>
correccion en libreria gen_excel, que escribia mal en la tabla core_history
</commit_message>
<xml_diff>
--- a/airflow/reports/reporte.xlsx
+++ b/airflow/reports/reporte.xlsx
@@ -553,7 +553,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>IC1.HOR1</t>
+          <t>IC1.SLO1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -563,12 +563,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>100GE2/0/0</t>
+          <t>100GE9/1/5</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/0</t>
+          <t>IC1.SLO1100GE9/1/5</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -588,7 +588,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/0)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/3/0/3) (S001_10 98SLO01 13/2) Linea:15009206</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -616,12 +616,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>100GE2/0/1</t>
+          <t>100GE2/0/0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/1</t>
+          <t>IC1.HOR1100GE2/0/0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/1)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/0)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -669,12 +669,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>100GE2/0/2</t>
+          <t>100GE2/0/1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/2</t>
+          <t>IC1.HOR1100GE2/0/1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/2)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/1)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -722,12 +722,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>100GE2/0/3</t>
+          <t>100GE2/0/2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/3</t>
+          <t>IC1.HOR1100GE2/0/2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/3)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/2)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -775,12 +775,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>100GE2/0/4</t>
+          <t>100GE2/0/3</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/4</t>
+          <t>IC1.HOR1100GE2/0/3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -800,7 +800,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/4)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/3)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -828,12 +828,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>100GE2/0/5</t>
+          <t>100GE2/0/4</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/5</t>
+          <t>IC1.HOR1100GE2/0/4</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/5)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/4)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -881,12 +881,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>100GE2/0/6</t>
+          <t>100GE2/0/5</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/6</t>
+          <t>IC1.HOR1100GE2/0/5</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/6)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/5)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -934,12 +934,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>100GE2/0/10</t>
+          <t>100GE2/0/6</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/10</t>
+          <t>IC1.HOR1100GE2/0/6</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/0)</t>
+          <t>TRK:ENLACE:ROC2.HOR1 (Hu0/11/0/6)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -987,12 +987,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>100GE2/0/11</t>
+          <t>100GE2/0/10</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/11</t>
+          <t>IC1.HOR1100GE2/0/10</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/0)</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -1040,12 +1040,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>100GE2/0/12</t>
+          <t>100GE2/0/11</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/12</t>
+          <t>IC1.HOR1100GE2/0/11</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/1)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
@@ -1093,12 +1093,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>100GE2/0/13</t>
+          <t>100GE2/0/12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/13</t>
+          <t>IC1.HOR1100GE2/0/12</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/3)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/2)</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>100GE2/0/14</t>
+          <t>100GE2/0/13</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/14</t>
+          <t>IC1.HOR1100GE2/0/13</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/0)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/1/0/3)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -1199,12 +1199,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>100GE2/0/15</t>
+          <t>100GE2/0/14</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/15</t>
+          <t>IC1.HOR1100GE2/0/14</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/0)</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -1252,12 +1252,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>100GE2/0/16</t>
+          <t>100GE2/0/15</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/16</t>
+          <t>IC1.HOR1100GE2/0/15</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/1)</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
@@ -1305,12 +1305,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>100GE2/0/17</t>
+          <t>100GE2/0/16</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/17</t>
+          <t>IC1.HOR1100GE2/0/16</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/3)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/2)</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -1358,12 +1358,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>100GE2/0/18</t>
+          <t>100GE2/0/17</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/18</t>
+          <t>IC1.HOR1100GE2/0/17</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/3/0/3)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/2/0/3)</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
@@ -1411,12 +1411,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>100GE2/0/19</t>
+          <t>100GE2/0/18</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/0/19</t>
+          <t>IC1.HOR1100GE2/0/18</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/0)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/3/0/3)</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -1464,12 +1464,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>100GE2/1/0</t>
+          <t>100GE2/0/19</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/0</t>
+          <t>IC1.HOR1100GE2/0/19</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/0)</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -1517,12 +1517,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>100GE2/1/1</t>
+          <t>100GE2/1/0</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/1</t>
+          <t>IC1.HOR1100GE2/1/0</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/1)</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -1570,12 +1570,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>100GE2/1/2</t>
+          <t>100GE2/1/1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/2</t>
+          <t>IC1.HOR1100GE2/1/1</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1595,7 +1595,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/3)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/2)</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
@@ -1623,12 +1623,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>100GE2/1/3</t>
+          <t>100GE2/1/2</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/3</t>
+          <t>IC1.HOR1100GE2/1/2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/0/0/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu1/7/0/3)</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -1676,12 +1676,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>100GE2/1/4</t>
+          <t>100GE2/1/3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/4</t>
+          <t>IC1.HOR1100GE2/1/3</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/0)</t>
+          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/0/0/1)</t>
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
@@ -1729,12 +1729,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>100GE2/1/5</t>
+          <t>100GE2/1/4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE2/1/5</t>
+          <t>IC1.HOR1100GE2/1/4</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1754,7 +1754,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/1)</t>
+          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/0)</t>
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
@@ -1782,12 +1782,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>100GE8/0/0</t>
+          <t>100GE2/1/5</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/0</t>
+          <t>IC1.HOR1100GE2/1/5</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/0) (S3-005 88HOR02 0/3/1) Linea:11004841</t>
+          <t>TRK:ENLACE:ROS6.HOR1 (Hu0/5/1/1)</t>
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
@@ -1835,12 +1835,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>100GE8/0/1</t>
+          <t>100GE8/0/0</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/1</t>
+          <t>IC1.HOR1100GE8/0/0</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/1) (S3-004 88HOR01 0/3/1) Linea:11004840</t>
+          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/0) (S3-005 88HOR02 0/3/1) Linea:11004841</t>
         </is>
       </c>
       <c r="J26" t="inlineStr"/>
@@ -1888,12 +1888,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>100GE8/0/2</t>
+          <t>100GE8/0/1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/2</t>
+          <t>IC1.HOR1100GE8/0/1</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/2) (S3-002 88HOR01 0/12/1) Linea:15003692</t>
+          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/1) (S3-004 88HOR01 0/3/1) Linea:11004840</t>
         </is>
       </c>
       <c r="J27" t="inlineStr"/>
@@ -1941,12 +1941,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>100GE8/0/3</t>
+          <t>100GE8/0/2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE8/0/3</t>
+          <t>IC1.HOR1100GE8/0/2</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:IRD1NA (Hu0/5/0/0) (S3-001 88HOR02 0/16/1) Linea:15003451</t>
+          <t>TRK:ENLACE:IRD1NA (Hu0/7/0/2) (S3-002 88HOR01 0/12/1) Linea:15003692</t>
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
@@ -1994,12 +1994,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>100GE9/0/0</t>
+          <t>100GE8/0/3</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/0</t>
+          <t>IC1.HOR1100GE8/0/3</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2019,14 +2019,10 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/2) (32WPU01 2/15/C2) Linea:15008585</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Linea:15008585</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:IRD1NA (Hu0/5/0/0) (S3-001 88HOR02 0/16/1) Linea:15003451</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
           <t>ok</t>
@@ -2051,12 +2047,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>100GE9/0/1</t>
+          <t>100GE9/0/0</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/1</t>
+          <t>IC1.HOR1100GE9/0/0</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2076,12 +2072,12 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/3) (32WPU01 2/15/C1) Linea:15008555</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/2) (32WPU01 2/15/C2) Linea:15008585</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Linea:15008555</t>
+          <t>Linea:15008585</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2108,12 +2104,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>100GE9/0/2</t>
+          <t>100GE9/0/1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/2</t>
+          <t>IC1.HOR1100GE9/0/1</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2133,12 +2129,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/4) (32WPU01 1/14/C1) Linea:15008586</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/3) (32WPU01 2/15/C1) Linea:15008555</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Linea:15008586</t>
+          <t>Linea:15008555</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2165,12 +2161,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>100GE9/0/3</t>
+          <t>100GE9/0/2</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/3</t>
+          <t>IC1.HOR1100GE9/0/2</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2190,12 +2186,12 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/5) (32WPU01 1/16/C1) Linea:15008587</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/4) (32WPU01 1/14/C1) Linea:15008586</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Linea:15008587</t>
+          <t>Linea:15008586</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2222,12 +2218,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>100GE9/0/4</t>
+          <t>100GE9/0/3</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/4</t>
+          <t>IC1.HOR1100GE9/0/3</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2247,12 +2243,12 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/9/0/6)  (32WPU01 1/16/C2) Linea:15008383</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/15/0/5) (32WPU01 1/16/C1) Linea:15008587</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Linea:15008383</t>
+          <t>Linea:15008587</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2279,12 +2275,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>100GE9/0/5</t>
+          <t>100GE9/0/4</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/5</t>
+          <t>IC1.HOR1100GE9/0/4</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2304,10 +2300,14 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/1) (S004_1 98HOR02 5/1)</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/9/0/6)  (32WPU01 1/16/C2) Linea:15008383</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Linea:15008383</t>
+        </is>
+      </c>
       <c r="K34" t="inlineStr">
         <is>
           <t>ok</t>
@@ -2332,12 +2332,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>100GE9/0/6</t>
+          <t>100GE9/0/5</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/6</t>
+          <t>IC1.HOR1100GE9/0/5</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/2) (S004_2 98HOR02 5/2)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/1) (S004_1 98HOR02 5/1)</t>
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
@@ -2385,12 +2385,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>100GE9/0/7</t>
+          <t>100GE9/0/6</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/7</t>
+          <t>IC1.HOR1100GE9/0/6</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/0) (S004_3 98HOR02 6/1)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/2/0/2) (S004_2 98HOR02 5/2)</t>
         </is>
       </c>
       <c r="J36" t="inlineStr"/>
@@ -2438,12 +2438,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>100GE9/0/8</t>
+          <t>100GE9/0/7</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/8</t>
+          <t>IC1.HOR1100GE9/0/7</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/1) (S004_4 98HOR02 6/2)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/0) (S004_3 98HOR02 6/1)</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
@@ -2491,12 +2491,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>100GE9/0/9</t>
+          <t>100GE9/0/8</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/9</t>
+          <t>IC1.HOR1100GE9/0/8</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2516,7 +2516,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/2) (S004_5 98HOR02 7/1)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/1) (S004_4 98HOR02 6/2)</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
@@ -2544,12 +2544,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>100GE9/0/10</t>
+          <t>100GE9/0/9</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/10</t>
+          <t>IC1.HOR1100GE9/0/9</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/2) (S004_6 98HOR02 7/2)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/4/0/2) (S004_5 98HOR02 7/1)</t>
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
@@ -2597,12 +2597,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>100GE9/0/11</t>
+          <t>100GE9/0/10</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/11</t>
+          <t>IC1.HOR1100GE9/0/10</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2622,7 +2622,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/3) (S004_7 98HOR02 8/1)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/2) (S004_6 98HOR02 7/2)</t>
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
@@ -2650,12 +2650,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>100GE9/0/12</t>
+          <t>100GE9/0/11</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/12</t>
+          <t>IC1.HOR1100GE9/0/11</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/4) (WDM3.HOR1 2/3/C1)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/5/0/3) (S004_7 98HOR02 8/1)</t>
         </is>
       </c>
       <c r="J41" t="inlineStr"/>
@@ -2703,12 +2703,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>100GE9/0/13</t>
+          <t>100GE9/0/12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/13</t>
+          <t>IC1.HOR1100GE9/0/12</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/5) (WDM3.HOR1 4/9/C1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/4) (WDM3.HOR1 2/3/C1)</t>
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
@@ -2756,12 +2756,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>100GE9/0/14</t>
+          <t>100GE9/0/13</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/14</t>
+          <t>IC1.HOR1100GE9/0/13</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2781,7 +2781,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/6) (WDM3.HOR1 4/11/C1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/5) (WDM3.HOR1 4/9/C1)</t>
         </is>
       </c>
       <c r="J43" t="inlineStr"/>
@@ -2809,12 +2809,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>100GE9/0/15</t>
+          <t>100GE9/0/14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/15</t>
+          <t>IC1.HOR1100GE9/0/14</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2834,7 +2834,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/3) (WDM3.HOR1 4/1/C1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/6/0/6) (WDM3.HOR1 4/11/C1)</t>
         </is>
       </c>
       <c r="J44" t="inlineStr"/>
@@ -2862,12 +2862,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>100GE9/0/16</t>
+          <t>100GE9/0/15</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/16</t>
+          <t>IC1.HOR1100GE9/0/15</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2887,7 +2887,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/4) (WDM3.HOR1 4/3/C1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/3) (WDM3.HOR1 4/1/C1)</t>
         </is>
       </c>
       <c r="J45" t="inlineStr"/>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>100GE9/0/17</t>
+          <t>100GE9/0/16</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/17</t>
+          <t>IC1.HOR1100GE9/0/16</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2940,7 +2940,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/5) (WDM3.HOR1 4/4/C1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/4) (WDM3.HOR1 4/3/C1)</t>
         </is>
       </c>
       <c r="J46" t="inlineStr"/>
@@ -2968,12 +2968,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>100GE9/0/18</t>
+          <t>100GE9/0/17</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/18</t>
+          <t>IC1.HOR1100GE9/0/17</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2993,7 +2993,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/8/0/3) (WDM3.HOR1 4/6/C1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/7/0/5) (WDM3.HOR1 4/4/C1)</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -3021,12 +3021,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>100GE9/0/19</t>
+          <t>100GE9/0/18</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/0/19</t>
+          <t>IC1.HOR1100GE9/0/18</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3046,7 +3046,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/0/0/11) (WDM3.HOR1 6/8/C2)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/8/0/3) (WDM3.HOR1 4/6/C1)</t>
         </is>
       </c>
       <c r="J48" t="inlineStr"/>
@@ -3074,12 +3074,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>100GE9/1/0</t>
+          <t>100GE9/0/19</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/0</t>
+          <t>IC1.HOR1100GE9/0/19</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -3099,7 +3099,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/0) (S006_1 98HOR01 1C/6/1)</t>
+          <t>TRK:ENLACE:ROC2.AVA1 (Hu0/0/0/11) (WDM3.HOR1 6/8/C2)</t>
         </is>
       </c>
       <c r="J49" t="inlineStr"/>
@@ -3127,12 +3127,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>100GE9/1/1</t>
+          <t>100GE9/1/0</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/1</t>
+          <t>IC1.HOR1100GE9/1/0</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3152,7 +3152,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/1) (S006_2 98HOR01 1C/6/2)</t>
+          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/0) (S006_1 98HOR01 1C/6/1)</t>
         </is>
       </c>
       <c r="J50" t="inlineStr"/>
@@ -3180,12 +3180,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>100GE9/1/2</t>
+          <t>100GE9/1/1</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/2</t>
+          <t>IC1.HOR1100GE9/1/1</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/1/0) (S006_3 98HOR01 1C/7/1)</t>
+          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/0/1) (S006_2 98HOR01 1C/6/2)</t>
         </is>
       </c>
       <c r="J51" t="inlineStr"/>
@@ -3233,12 +3233,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>100GE9/1/3</t>
+          <t>100GE9/1/2</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/3</t>
+          <t>IC1.HOR1100GE9/1/2</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -3258,14 +3258,10 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/0) (S004_8 98HOR02 8/2) Linea:15009213</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Linea:15009213</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROS6.SLO1 (Hu0/5/1/0) (S006_3 98HOR01 1C/7/1)</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3290,12 +3286,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>100GE9/1/4</t>
+          <t>100GE9/1/3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/4</t>
+          <t>IC1.HOR1100GE9/1/3</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -3315,12 +3311,12 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/1) (S004_9 98HOR02 14/1) Linea:15009214</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/0) (S004_8 98HOR02 8/2) Linea:15009213</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Linea:15009214</t>
+          <t>Linea:15009213</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -3347,12 +3343,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>100GE9/1/5</t>
+          <t>100GE9/1/4</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/5</t>
+          <t>IC1.HOR1100GE9/1/4</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -3372,12 +3368,12 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/2) (S004_10 98HOR02 14/2) Linea:15009215</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/1) (S004_9 98HOR02 14/1) Linea:15009214</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Linea:15009215</t>
+          <t>Linea:15009214</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -3404,12 +3400,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>100GE9/1/6</t>
+          <t>100GE9/1/5</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/6</t>
+          <t>IC1.HOR1100GE9/1/5</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -3429,12 +3425,12 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/2) (98HOR01 3/1) Linea: 15009094</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu0/7/0/2) (S004_10 98HOR02 14/2) Linea:15009215</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Linea: 15009094</t>
+          <t>Linea:15009215</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -3461,12 +3457,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>100GE9/1/7</t>
+          <t>100GE9/1/6</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/7</t>
+          <t>IC1.HOR1100GE9/1/6</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -3486,12 +3482,12 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/3) (98HOR01 3/2) Linea: 15009095</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/2) (98HOR01 3/1) Linea: 15009094</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Linea: 15009095</t>
+          <t>Linea: 15009094</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -3518,12 +3514,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>100GE9/1/8</t>
+          <t>100GE9/1/7</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/8</t>
+          <t>IC1.HOR1100GE9/1/7</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -3543,12 +3539,12 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/4) (98HOR01 5/1) Linea: 15009096</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/3) (98HOR01 3/2) Linea: 15009095</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Linea: 15009096 - BEL1NA</t>
+          <t>Linea: 15009095</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -3575,12 +3571,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>100GE9/1/9</t>
+          <t>100GE9/1/8</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/9</t>
+          <t>IC1.HOR1100GE9/1/8</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -3600,12 +3596,12 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/5) (98HOR01 5/2) Linea: 15009097</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/4) (98HOR01 5/1) Linea: 15009096</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Linea: 15009097 - BEL1NA</t>
+          <t>Linea: 15009096 - BEL1NA</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -3632,12 +3628,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>100GE9/1/10</t>
+          <t>100GE9/1/9</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>IC1.HOR1100GE9/1/10</t>
+          <t>IC1.HOR1100GE9/1/9</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -3657,12 +3653,12 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/6) (98HOR01 4/1) Linea: 15009098</t>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/5) (98HOR01 5/2) Linea: 15009097</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Linea: 15009098</t>
+          <t>Linea: 15009097 - BEL1NA</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -3679,7 +3675,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>IC1.SLO1</t>
+          <t>IC1.HOR1</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3689,12 +3685,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>100GE2/0/0</t>
+          <t>100GE9/1/10</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/0</t>
+          <t>IC1.HOR1100GE9/1/10</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -3714,10 +3710,14 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/0)</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr"/>
+          <t>TRK:ENLACE:BEL1NA (Hu0/17/0/6) (98HOR01 4/1) Linea: 15009098</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Linea: 15009098</t>
+        </is>
+      </c>
       <c r="K60" t="inlineStr">
         <is>
           <t>ok</t>
@@ -3742,12 +3742,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>100GE2/0/1</t>
+          <t>100GE2/0/0</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/1</t>
+          <t>IC1.SLO1100GE2/0/0</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -3767,7 +3767,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/1)</t>
+          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/0)</t>
         </is>
       </c>
       <c r="J61" t="inlineStr"/>
@@ -3795,12 +3795,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>100GE2/0/2</t>
+          <t>100GE2/0/1</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/2</t>
+          <t>IC1.SLO1100GE2/0/1</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/2)</t>
+          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/1)</t>
         </is>
       </c>
       <c r="J62" t="inlineStr"/>
@@ -3848,12 +3848,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>100GE2/0/3</t>
+          <t>100GE2/0/2</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/3</t>
+          <t>IC1.SLO1100GE2/0/2</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/3)</t>
+          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/2)</t>
         </is>
       </c>
       <c r="J63" t="inlineStr"/>
@@ -3901,12 +3901,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>100GE2/0/4</t>
+          <t>100GE2/0/3</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/4</t>
+          <t>IC1.SLO1100GE2/0/3</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3926,7 +3926,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/4)</t>
+          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/3)</t>
         </is>
       </c>
       <c r="J64" t="inlineStr"/>
@@ -3954,12 +3954,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>100GE2/0/5</t>
+          <t>100GE2/0/4</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/5</t>
+          <t>IC1.SLO1100GE2/0/4</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3979,7 +3979,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/5)</t>
+          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/4)</t>
         </is>
       </c>
       <c r="J65" t="inlineStr"/>
@@ -4007,12 +4007,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>100GE2/0/6</t>
+          <t>100GE2/0/5</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/6</t>
+          <t>IC1.SLO1100GE2/0/5</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -4032,7 +4032,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/6)</t>
+          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/5)</t>
         </is>
       </c>
       <c r="J66" t="inlineStr"/>
@@ -4060,12 +4060,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>100GE2/0/7</t>
+          <t>100GE2/0/6</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/7</t>
+          <t>IC1.SLO1100GE2/0/6</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -4085,7 +4085,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/7)</t>
+          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/6)</t>
         </is>
       </c>
       <c r="J67" t="inlineStr"/>
@@ -4113,12 +4113,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>100GE2/0/11</t>
+          <t>100GE2/0/7</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/11</t>
+          <t>IC1.SLO1100GE2/0/7</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -4138,7 +4138,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/1/0/3)</t>
+          <t>TRK:ENLACE:ROC2.SLO1 (Hu0/11/0/7)</t>
         </is>
       </c>
       <c r="J68" t="inlineStr"/>
@@ -4166,12 +4166,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>100GE2/0/12</t>
+          <t>100GE2/0/11</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/12</t>
+          <t>IC1.SLO1100GE2/0/11</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -4191,7 +4191,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/3/0/2)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/1/0/3)</t>
         </is>
       </c>
       <c r="J69" t="inlineStr"/>
@@ -4219,12 +4219,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>100GE2/0/13</t>
+          <t>100GE2/0/12</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/13</t>
+          <t>IC1.SLO1100GE2/0/12</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -4244,7 +4244,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/3/0/3)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/3/0/2)</t>
         </is>
       </c>
       <c r="J70" t="inlineStr"/>
@@ -4272,12 +4272,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>100GE2/0/14</t>
+          <t>100GE2/0/13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/14</t>
+          <t>IC1.SLO1100GE2/0/13</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -4297,7 +4297,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/4/0/0)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/3/0/3)</t>
         </is>
       </c>
       <c r="J71" t="inlineStr"/>
@@ -4325,12 +4325,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>100GE2/0/15</t>
+          <t>100GE2/0/14</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/15</t>
+          <t>IC1.SLO1100GE2/0/14</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/4/0/1)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/4/0/0)</t>
         </is>
       </c>
       <c r="J72" t="inlineStr"/>
@@ -4378,12 +4378,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>100GE2/0/16</t>
+          <t>100GE2/0/15</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/16</t>
+          <t>IC1.SLO1100GE2/0/15</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -4403,7 +4403,7 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/4/0/2)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/4/0/1)</t>
         </is>
       </c>
       <c r="J73" t="inlineStr"/>
@@ -4431,12 +4431,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>100GE2/0/17</t>
+          <t>100GE2/0/16</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/17</t>
+          <t>IC1.SLO1100GE2/0/16</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -4456,7 +4456,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/4/0/3)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/4/0/2)</t>
         </is>
       </c>
       <c r="J74" t="inlineStr"/>
@@ -4484,12 +4484,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>100GE2/0/18</t>
+          <t>100GE2/0/17</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/18</t>
+          <t>IC1.SLO1100GE2/0/17</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -4509,7 +4509,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/5/0/0)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/4/0/3)</t>
         </is>
       </c>
       <c r="J75" t="inlineStr"/>
@@ -4537,12 +4537,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>100GE2/0/19</t>
+          <t>100GE2/0/18</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/0/19</t>
+          <t>IC1.SLO1100GE2/0/18</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -4562,7 +4562,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/5/0/1)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/5/0/0)</t>
         </is>
       </c>
       <c r="J76" t="inlineStr"/>
@@ -4590,12 +4590,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>100GE2/1/0</t>
+          <t>100GE2/0/19</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/1/0</t>
+          <t>IC1.SLO1100GE2/0/19</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -4615,7 +4615,7 @@
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/5/0/2)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/5/0/1)</t>
         </is>
       </c>
       <c r="J77" t="inlineStr"/>
@@ -4643,12 +4643,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>100GE2/1/1</t>
+          <t>100GE2/1/0</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/1/1</t>
+          <t>IC1.SLO1100GE2/1/0</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -4668,7 +4668,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/5/0/3)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/5/0/2)</t>
         </is>
       </c>
       <c r="J78" t="inlineStr"/>
@@ -4696,12 +4696,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>100GE2/1/2</t>
+          <t>100GE2/1/1</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/1/2</t>
+          <t>IC1.SLO1100GE2/1/1</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/7/0/2)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/5/0/3)</t>
         </is>
       </c>
       <c r="J79" t="inlineStr"/>
@@ -4749,12 +4749,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>100GE2/1/3</t>
+          <t>100GE2/1/2</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/1/3</t>
+          <t>IC1.SLO1100GE2/1/2</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -4774,7 +4774,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/7/0/3)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/7/0/2)</t>
         </is>
       </c>
       <c r="J80" t="inlineStr"/>
@@ -4802,12 +4802,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>100GE2/1/4</t>
+          <t>100GE2/1/3</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/1/4</t>
+          <t>IC1.SLO1100GE2/1/3</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -4827,7 +4827,7 @@
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS7.SLO1 (Hu0/5/0/0)</t>
+          <t>TRK:ENLACE:ROE1.SLO1 (Hu1/7/0/3)</t>
         </is>
       </c>
       <c r="J81" t="inlineStr"/>
@@ -4855,12 +4855,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>100GE2/1/5</t>
+          <t>100GE2/1/4</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/1/5</t>
+          <t>IC1.SLO1100GE2/1/4</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -4880,7 +4880,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS7.SLO1 (Hu0/5/0/1)</t>
+          <t>TRK:ENLACE:ROS7.SLO1 (Hu0/5/0/0)</t>
         </is>
       </c>
       <c r="J82" t="inlineStr"/>
@@ -4908,12 +4908,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>100GE2/1/6</t>
+          <t>100GE2/1/5</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE2/1/6</t>
+          <t>IC1.SLO1100GE2/1/5</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS7.SLO1 (Hu0/5/1/0)</t>
+          <t>TRK:ENLACE:ROS7.SLO1 (Hu0/5/0/1)</t>
         </is>
       </c>
       <c r="J83" t="inlineStr"/>
@@ -4961,12 +4961,12 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>100GE9/0/0</t>
+          <t>100GE2/1/6</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/0</t>
+          <t>IC1.SLO1100GE2/1/6</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -4986,14 +4986,10 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/0) (32FIB01 2/15/C2) Linea:15008588</t>
-        </is>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>15008588</t>
-        </is>
-      </c>
+          <t>TRK:ENLACE:ROS7.SLO1 (Hu0/5/1/0)</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr">
         <is>
           <t>ok</t>
@@ -5018,12 +5014,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>100GE9/0/1</t>
+          <t>100GE9/0/0</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/1</t>
+          <t>IC1.SLO1100GE9/0/0</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -5043,12 +5039,12 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/1) (32FIB01 2/15/C1) Linea:15008589</t>
+          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/0) (32FIB01 2/15/C2) Linea:15008588</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>15008589</t>
+          <t>15008588</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -5075,12 +5071,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>100GE9/0/2</t>
+          <t>100GE9/0/1</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/2</t>
+          <t>IC1.SLO1100GE9/0/1</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -5100,12 +5096,12 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/2) (32FIB01 2/7/C1)  Linea:15008590</t>
+          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/1) (32FIB01 2/15/C1) Linea:15008589</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>15008590</t>
+          <t>15008589</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -5132,12 +5128,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>100GE9/0/3</t>
+          <t>100GE9/0/2</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/3</t>
+          <t>IC1.SLO1100GE9/0/2</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -5157,12 +5153,12 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/3) (32FIB01 1/16/C1) Linea:15008554</t>
+          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/2) (32FIB01 2/7/C1)  Linea:15008590</t>
         </is>
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>15008554</t>
+          <t>15008590</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -5189,12 +5185,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>100GE9/0/4</t>
+          <t>100GE9/0/3</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/4</t>
+          <t>IC1.SLO1100GE9/0/3</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -5214,12 +5210,12 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/5) (32FIB01 1/16/C2) Linea:15008382</t>
+          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/3) (32FIB01 1/16/C1) Linea:15008554</t>
         </is>
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>15008382</t>
+          <t>15008554</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -5246,12 +5242,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>100GE9/0/5</t>
+          <t>100GE9/0/4</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/5</t>
+          <t>IC1.SLO1100GE9/0/4</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -5271,10 +5267,14 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/0/0/0) (S001_1 98SLO01 1/1)</t>
-        </is>
-      </c>
-      <c r="J89" t="inlineStr"/>
+          <t>TRK:ENLACE:MUN1NA (Hu0/15/0/5) (32FIB01 1/16/C2) Linea:15008382</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>15008382</t>
+        </is>
+      </c>
       <c r="K89" t="inlineStr">
         <is>
           <t>ok</t>
@@ -5299,12 +5299,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>100GE9/0/6</t>
+          <t>100GE9/0/5</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/6</t>
+          <t>IC1.SLO1100GE9/0/5</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -5324,7 +5324,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/0/0/1) (S001_2 98SLO01 1/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/0/0/0) (S001_1 98SLO01 1/1)</t>
         </is>
       </c>
       <c r="J90" t="inlineStr"/>
@@ -5352,12 +5352,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>100GE9/0/7</t>
+          <t>100GE9/0/6</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/7</t>
+          <t>IC1.SLO1100GE9/0/6</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/2/0/1) (S001_3 98SLO01 2/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/0/0/1) (S001_2 98SLO01 1/2)</t>
         </is>
       </c>
       <c r="J91" t="inlineStr"/>
@@ -5405,12 +5405,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>100GE9/0/8</t>
+          <t>100GE9/0/7</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/8</t>
+          <t>IC1.SLO1100GE9/0/7</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -5430,7 +5430,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/2/0/2) (S001_4 98SLO01 2/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/2/0/1) (S001_3 98SLO01 2/1)</t>
         </is>
       </c>
       <c r="J92" t="inlineStr"/>
@@ -5458,12 +5458,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>100GE9/0/9</t>
+          <t>100GE9/0/8</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/9</t>
+          <t>IC1.SLO1100GE9/0/8</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -5483,7 +5483,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/4/0/0) (S001_5 98SLO01 3/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/2/0/2) (S001_4 98SLO01 2/2)</t>
         </is>
       </c>
       <c r="J93" t="inlineStr"/>
@@ -5511,12 +5511,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>100GE9/0/10</t>
+          <t>100GE9/0/9</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/10</t>
+          <t>IC1.SLO1100GE9/0/9</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -5536,7 +5536,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/6/0/0) (S001_6 98SLO01 3/2)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/4/0/0) (S001_5 98SLO01 3/1)</t>
         </is>
       </c>
       <c r="J94" t="inlineStr"/>
@@ -5564,12 +5564,12 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>100GE9/0/11</t>
+          <t>100GE9/0/10</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/11</t>
+          <t>IC1.SLO1100GE9/0/10</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -5589,7 +5589,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/6/0/3) (S001_7 98SLO01 4/1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/6/0/0) (S001_6 98SLO01 3/2)</t>
         </is>
       </c>
       <c r="J95" t="inlineStr"/>
@@ -5617,12 +5617,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>100GE9/0/12</t>
+          <t>100GE9/0/11</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/12</t>
+          <t>IC1.SLO1100GE9/0/11</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -5642,7 +5642,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/0) (WDM3.SLO1 5/6/C1)</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/6/0/3) (S001_7 98SLO01 4/1)</t>
         </is>
       </c>
       <c r="J96" t="inlineStr"/>
@@ -5670,12 +5670,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>100GE9/0/13</t>
+          <t>100GE9/0/12</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/13</t>
+          <t>IC1.SLO1100GE9/0/12</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -5695,7 +5695,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/1) (WDM3.SLO1 5/9/C1)</t>
+          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/0) (WDM3.SLO1 5/6/C1)</t>
         </is>
       </c>
       <c r="J97" t="inlineStr"/>
@@ -5723,12 +5723,12 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>100GE9/0/14</t>
+          <t>100GE9/0/13</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/14</t>
+          <t>IC1.SLO1100GE9/0/13</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -5748,7 +5748,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/2) (WDM3.SLO1 5/11/C1)</t>
+          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/1) (WDM3.SLO1 5/9/C1)</t>
         </is>
       </c>
       <c r="J98" t="inlineStr"/>
@@ -5776,12 +5776,12 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>100GE9/0/15</t>
+          <t>100GE9/0/14</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/15</t>
+          <t>IC1.SLO1100GE9/0/14</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -5801,7 +5801,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/3) (WDM3.SLO1 5/1/C1)</t>
+          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/2) (WDM3.SLO1 5/11/C1)</t>
         </is>
       </c>
       <c r="J99" t="inlineStr"/>
@@ -5829,12 +5829,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>100GE9/0/16</t>
+          <t>100GE9/0/15</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/16</t>
+          <t>IC1.SLO1100GE9/0/15</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -5854,7 +5854,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/4) (WDM3.SLO1 5/3/C1)</t>
+          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/3) (WDM3.SLO1 5/1/C1)</t>
         </is>
       </c>
       <c r="J100" t="inlineStr"/>
@@ -5882,12 +5882,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>100GE9/0/17</t>
+          <t>100GE9/0/16</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/17</t>
+          <t>IC1.SLO1100GE9/0/16</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -5907,7 +5907,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/5) (WDM3.SLO1 5/4/C1)</t>
+          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/4) (WDM3.SLO1 5/3/C1)</t>
         </is>
       </c>
       <c r="J101" t="inlineStr"/>
@@ -5935,12 +5935,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>100GE9/0/18</t>
+          <t>100GE9/0/17</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/18</t>
+          <t>IC1.SLO1100GE9/0/17</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -5960,7 +5960,7 @@
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/6) (WDM3.SLO1 5/12/C1)</t>
+          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/5) (WDM3.SLO1 5/4/C1)</t>
         </is>
       </c>
       <c r="J102" t="inlineStr"/>
@@ -5988,12 +5988,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>100GE9/0/19</t>
+          <t>100GE9/0/18</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/0/19</t>
+          <t>IC1.SLO1100GE9/0/18</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS7.HOR1 (Hu0/0/0/1) (S003_1 98SLO02 2C/1/1)</t>
+          <t>TRK:ENLACE:ROC2.BEL1 (Hu0/9/0/6) (WDM3.SLO1 5/12/C1)</t>
         </is>
       </c>
       <c r="J103" t="inlineStr"/>
@@ -6041,12 +6041,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>100GE9/1/0</t>
+          <t>100GE9/0/19</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/1/0</t>
+          <t>IC1.SLO1100GE9/0/19</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -6066,7 +6066,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS7.HOR1 (Hu0/5/1/0) (S003_2 98SLO02 2C/1/2)</t>
+          <t>TRK:ENLACE:ROS7.HOR1 (Hu0/0/0/1) (S003_1 98SLO02 2C/1/1)</t>
         </is>
       </c>
       <c r="J104" t="inlineStr"/>
@@ -6094,12 +6094,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>100GE9/1/1</t>
+          <t>100GE9/1/0</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/1/1</t>
+          <t>IC1.SLO1100GE9/1/0</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -6119,7 +6119,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROS7.HOR1 (Hu0/5/1/1) (S003_3 98SLO02 2C/2/1)</t>
+          <t>TRK:ENLACE:ROS7.HOR1 (Hu0/5/1/0) (S003_2 98SLO02 2C/1/2)</t>
         </is>
       </c>
       <c r="J105" t="inlineStr"/>
@@ -6147,12 +6147,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>100GE9/1/3</t>
+          <t>100GE9/1/1</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/1/3</t>
+          <t>IC1.SLO1100GE9/1/1</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -6172,7 +6172,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/1/0/3) (S001_8 98SLO01 4/2) Linea:15009204</t>
+          <t>TRK:ENLACE:ROS7.HOR1 (Hu0/5/1/1) (S003_3 98SLO02 2C/2/1)</t>
         </is>
       </c>
       <c r="J106" t="inlineStr"/>
@@ -6200,12 +6200,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>100GE9/1/4</t>
+          <t>100GE9/1/3</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/1/4</t>
+          <t>IC1.SLO1100GE9/1/3</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -6225,7 +6225,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/2/0/3) (S001_9 98SLO01 13/1) Linea:15009205</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/1/0/3) (S001_8 98SLO01 4/2) Linea:15009204</t>
         </is>
       </c>
       <c r="J107" t="inlineStr"/>
@@ -6253,12 +6253,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>100GE9/1/5</t>
+          <t>100GE9/1/4</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>IC1.SLO1100GE9/1/5</t>
+          <t>IC1.SLO1100GE9/1/4</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -6278,7 +6278,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/3/0/3) (S001_10 98SLO01 13/2) Linea:15009206</t>
+          <t>TRK:ENLACE:ROE1.HOR1 (Hu0/2/0/3) (S001_9 98SLO01 13/1) Linea:15009205</t>
         </is>
       </c>
       <c r="J108" t="inlineStr"/>

</xml_diff>